<commit_message>
continued migration some refactoring added undoSimulationMove added vectorPool
</commit_message>
<xml_diff>
--- a/docs/Performance.xlsx
+++ b/docs/Performance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\Chess\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\clace\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1B5F11C-1EE4-47D3-AF76-912C01ED0DDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{032B937C-F9BF-412D-AB18-05593EF2EC61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1890" yWindow="2640" windowWidth="28800" windowHeight="15345" xr2:uid="{D3276BA4-EC86-47CC-ADFB-EDF16C1A358E}"/>
+    <workbookView xWindow="38280" yWindow="5280" windowWidth="29040" windowHeight="15720" xr2:uid="{D3276BA4-EC86-47CC-ADFB-EDF16C1A358E}"/>
   </bookViews>
   <sheets>
     <sheet name="Initial Position Single Thread" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>moves</t>
   </si>
@@ -65,6 +65,21 @@
   </si>
   <si>
     <t>vs target (80M)</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>porting c++ piu' qualche miglioria</t>
+  </si>
+  <si>
+    <t>undo simulation move</t>
+  </si>
+  <si>
+    <t>miglioria nella moves generator</t>
+  </si>
+  <si>
+    <t>vector pool</t>
   </si>
 </sst>
 </file>
@@ -74,7 +89,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d/mmm/yyyy;@"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,8 +127,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -130,8 +152,13 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -223,13 +250,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -255,13 +294,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="2" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="5" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="5" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -270,9 +316,13 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Good" xfId="3" builtinId="26"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -586,10 +636,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D63397-ACCF-47C4-BDCB-8082DFD2DBBB}">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:P20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,27 +649,30 @@
     <col min="8" max="8" width="16.140625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="10"/>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="17" t="s">
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="P1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
@@ -663,7 +716,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>45404</v>
       </c>
@@ -703,7 +756,7 @@
         <v>-0.96022560483870967</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B4" s="12"/>
       <c r="C4">
         <v>5</v>
@@ -738,6 +791,474 @@
       <c r="N4" s="8">
         <f>(L4-80000000)/80000000</f>
         <v>-0.93544281746031754</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="13">
+        <v>45553</v>
+      </c>
+      <c r="B6" s="14"/>
+      <c r="C6" s="19">
+        <v>4</v>
+      </c>
+      <c r="D6" s="15">
+        <v>206603</v>
+      </c>
+      <c r="E6" s="20">
+        <v>909</v>
+      </c>
+      <c r="F6" s="15">
+        <f>D6/E6*1000</f>
+        <v>227286.02860286029</v>
+      </c>
+      <c r="G6" s="18">
+        <f>(E3-E6)/E3</f>
+        <v>0.17363636363636364</v>
+      </c>
+      <c r="H6" s="16">
+        <f>(F6-80000000)/80000000</f>
+        <v>-0.99715892464246436</v>
+      </c>
+      <c r="I6" s="3">
+        <v>4</v>
+      </c>
+      <c r="J6" s="15">
+        <v>197281</v>
+      </c>
+      <c r="K6" s="3">
+        <v>48</v>
+      </c>
+      <c r="L6" s="15">
+        <f>J6/K6*1000</f>
+        <v>4110020.833333333</v>
+      </c>
+      <c r="M6" s="18">
+        <f>(K3-K6)/K3</f>
+        <v>0.22580645161290322</v>
+      </c>
+      <c r="N6" s="16">
+        <f>(L6-80000000)/80000000</f>
+        <v>-0.94862473958333338</v>
+      </c>
+      <c r="P6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>5072212</v>
+      </c>
+      <c r="E7">
+        <v>34300</v>
+      </c>
+      <c r="F7" s="4">
+        <f>D7/E7*1000</f>
+        <v>147877.90087463558</v>
+      </c>
+      <c r="G7" s="17">
+        <f>(E4-E7)/E4</f>
+        <v>0.18333333333333332</v>
+      </c>
+      <c r="H7" s="8">
+        <f>(F7-80000000)/80000000</f>
+        <v>-0.99815152623906711</v>
+      </c>
+      <c r="I7">
+        <v>5</v>
+      </c>
+      <c r="J7" s="4">
+        <v>4880523</v>
+      </c>
+      <c r="K7">
+        <v>727</v>
+      </c>
+      <c r="L7" s="4">
+        <f>J7/K7*1000</f>
+        <v>6713236.5887207706</v>
+      </c>
+      <c r="M7" s="17">
+        <f>(K4-K7)/K4</f>
+        <v>0.23068783068783069</v>
+      </c>
+      <c r="N7" s="8">
+        <f>(L7-80000000)/80000000</f>
+        <v>-0.91608454264099037</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I8">
+        <v>6</v>
+      </c>
+      <c r="J8" s="4">
+        <v>119060324</v>
+      </c>
+      <c r="K8">
+        <v>29235</v>
+      </c>
+      <c r="L8" s="4">
+        <f>J8/K8*1000</f>
+        <v>4072526.9026851379</v>
+      </c>
+      <c r="N8" s="8">
+        <f>(L8-80000000)/80000000</f>
+        <v>-0.94909341371643585</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="13">
+        <v>45554</v>
+      </c>
+      <c r="B10" s="14"/>
+      <c r="C10" s="19">
+        <v>4</v>
+      </c>
+      <c r="D10" s="15">
+        <v>206603</v>
+      </c>
+      <c r="E10" s="20">
+        <v>822</v>
+      </c>
+      <c r="F10" s="15">
+        <f>D10/E10*1000</f>
+        <v>251341.84914841849</v>
+      </c>
+      <c r="G10" s="18">
+        <f>(E6-E10)/E6</f>
+        <v>9.5709570957095716E-2</v>
+      </c>
+      <c r="H10" s="16">
+        <f>(F10-80000000)/80000000</f>
+        <v>-0.99685822688564474</v>
+      </c>
+      <c r="I10" s="3">
+        <v>4</v>
+      </c>
+      <c r="J10" s="15">
+        <v>197281</v>
+      </c>
+      <c r="K10" s="3">
+        <v>42</v>
+      </c>
+      <c r="L10" s="15">
+        <f>J10/K10*1000</f>
+        <v>4697166.666666667</v>
+      </c>
+      <c r="M10" s="18">
+        <f>(K6-K10)/K6</f>
+        <v>0.125</v>
+      </c>
+      <c r="N10" s="16">
+        <f>(L10-80000000)/80000000</f>
+        <v>-0.94128541666666665</v>
+      </c>
+      <c r="P10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="D11">
+        <v>5072212</v>
+      </c>
+      <c r="E11">
+        <v>30566</v>
+      </c>
+      <c r="F11" s="4">
+        <f>D11/E11*1000</f>
+        <v>165942.94313943599</v>
+      </c>
+      <c r="G11" s="17">
+        <f>(E7-E11)/E7</f>
+        <v>0.10886297376093294</v>
+      </c>
+      <c r="H11" s="8">
+        <f>(F11-80000000)/80000000</f>
+        <v>-0.99792571321075707</v>
+      </c>
+      <c r="I11">
+        <v>5</v>
+      </c>
+      <c r="J11" s="4">
+        <v>4880523</v>
+      </c>
+      <c r="K11">
+        <v>631</v>
+      </c>
+      <c r="L11" s="4">
+        <f>J11/K11*1000</f>
+        <v>7734584.7860538829</v>
+      </c>
+      <c r="M11" s="17">
+        <f>(K7-K11)/K7</f>
+        <v>0.13204951856946354</v>
+      </c>
+      <c r="N11" s="8">
+        <f>(L11-80000000)/80000000</f>
+        <v>-0.9033176901743265</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I12">
+        <v>6</v>
+      </c>
+      <c r="J12" s="4">
+        <v>119060324</v>
+      </c>
+      <c r="K12">
+        <v>25861</v>
+      </c>
+      <c r="L12" s="4">
+        <f>J12/K12*1000</f>
+        <v>4603856.1540543679</v>
+      </c>
+      <c r="M12" s="17">
+        <f>(K8-K12)/K8</f>
+        <v>0.11540961176671798</v>
+      </c>
+      <c r="N12" s="8">
+        <f>(L12-80000000)/80000000</f>
+        <v>-0.94245179807432033</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="13">
+        <v>45557</v>
+      </c>
+      <c r="B14" s="14"/>
+      <c r="C14" s="19">
+        <v>4</v>
+      </c>
+      <c r="D14" s="15">
+        <v>206603</v>
+      </c>
+      <c r="E14" s="20">
+        <v>778</v>
+      </c>
+      <c r="F14" s="15">
+        <f>D14/E14*1000</f>
+        <v>265556.55526992283</v>
+      </c>
+      <c r="G14" s="18">
+        <f>(E10-E14)/E10</f>
+        <v>5.3527980535279802E-2</v>
+      </c>
+      <c r="H14" s="16">
+        <f>(F14-80000000)/80000000</f>
+        <v>-0.9966805430591259</v>
+      </c>
+      <c r="I14" s="3">
+        <v>4</v>
+      </c>
+      <c r="J14" s="15">
+        <v>197281</v>
+      </c>
+      <c r="K14" s="3">
+        <v>42</v>
+      </c>
+      <c r="L14" s="15">
+        <f>J14/K14*1000</f>
+        <v>4697166.666666667</v>
+      </c>
+      <c r="M14" s="18">
+        <f>(K10-K14)/K10</f>
+        <v>0</v>
+      </c>
+      <c r="N14" s="16">
+        <f>(L14-80000000)/80000000</f>
+        <v>-0.94128541666666665</v>
+      </c>
+      <c r="P14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>5</v>
+      </c>
+      <c r="D15">
+        <v>5072212</v>
+      </c>
+      <c r="E15">
+        <v>30233</v>
+      </c>
+      <c r="F15" s="4">
+        <f>D15/E15*1000</f>
+        <v>167770.71412033209</v>
+      </c>
+      <c r="G15" s="17">
+        <f>(E11-E15)/E11</f>
+        <v>1.0894457894392463E-2</v>
+      </c>
+      <c r="H15" s="8">
+        <f>(F15-80000000)/80000000</f>
+        <v>-0.99790286607349588</v>
+      </c>
+      <c r="I15">
+        <v>5</v>
+      </c>
+      <c r="J15" s="4">
+        <v>4880523</v>
+      </c>
+      <c r="K15">
+        <v>570</v>
+      </c>
+      <c r="L15" s="4">
+        <f>J15/K15*1000</f>
+        <v>8562321.0526315793</v>
+      </c>
+      <c r="M15" s="17">
+        <f>(K11-K15)/K11</f>
+        <v>9.6671949286846276E-2</v>
+      </c>
+      <c r="N15" s="8">
+        <f>(L15-80000000)/80000000</f>
+        <v>-0.89297098684210519</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I16">
+        <v>6</v>
+      </c>
+      <c r="J16" s="4">
+        <v>119060324</v>
+      </c>
+      <c r="K16">
+        <v>25569</v>
+      </c>
+      <c r="L16" s="4">
+        <f>J16/K16*1000</f>
+        <v>4656432.5550471274</v>
+      </c>
+      <c r="M16" s="17">
+        <f>(K12-K16)/K12</f>
+        <v>1.129113336684583E-2</v>
+      </c>
+      <c r="N16" s="8">
+        <f>(L16-80000000)/80000000</f>
+        <v>-0.94179459306191093</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" s="13">
+        <v>45559</v>
+      </c>
+      <c r="B18" s="14"/>
+      <c r="C18" s="19">
+        <v>4</v>
+      </c>
+      <c r="D18" s="15">
+        <v>206603</v>
+      </c>
+      <c r="E18" s="20">
+        <v>648</v>
+      </c>
+      <c r="F18" s="15">
+        <f>D18/E18*1000</f>
+        <v>318831.7901234568</v>
+      </c>
+      <c r="G18" s="18">
+        <f>(E14-E18)/E14</f>
+        <v>0.16709511568123395</v>
+      </c>
+      <c r="H18" s="16">
+        <f>(F18-80000000)/80000000</f>
+        <v>-0.99601460262345676</v>
+      </c>
+      <c r="I18" s="3">
+        <v>4</v>
+      </c>
+      <c r="J18" s="15">
+        <v>197281</v>
+      </c>
+      <c r="K18" s="3">
+        <v>17</v>
+      </c>
+      <c r="L18" s="15">
+        <f>J18/K18*1000</f>
+        <v>11604764.705882354</v>
+      </c>
+      <c r="M18" s="18">
+        <f>(K14-K18)/K14</f>
+        <v>0.59523809523809523</v>
+      </c>
+      <c r="N18" s="16">
+        <f>(L18-80000000)/80000000</f>
+        <v>-0.8549404411764705</v>
+      </c>
+      <c r="P18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>5</v>
+      </c>
+      <c r="D19">
+        <v>5072212</v>
+      </c>
+      <c r="E19">
+        <v>15906</v>
+      </c>
+      <c r="F19" s="4">
+        <f>D19/E19*1000</f>
+        <v>318886.70941782976</v>
+      </c>
+      <c r="G19" s="17">
+        <f>(E15-E19)/E15</f>
+        <v>0.47388615089471769</v>
+      </c>
+      <c r="H19" s="8">
+        <f>(F19-80000000)/80000000</f>
+        <v>-0.99601391613227708</v>
+      </c>
+      <c r="I19">
+        <v>5</v>
+      </c>
+      <c r="J19" s="4">
+        <v>4880523</v>
+      </c>
+      <c r="K19">
+        <v>441</v>
+      </c>
+      <c r="L19" s="4">
+        <f>J19/K19*1000</f>
+        <v>11066945.578231292</v>
+      </c>
+      <c r="M19" s="17">
+        <f>(K15-K19)/K15</f>
+        <v>0.22631578947368422</v>
+      </c>
+      <c r="N19" s="8">
+        <f>(L19-80000000)/80000000</f>
+        <v>-0.86166318027210886</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I20">
+        <v>6</v>
+      </c>
+      <c r="J20" s="4">
+        <v>119060324</v>
+      </c>
+      <c r="K20">
+        <v>10853</v>
+      </c>
+      <c r="L20" s="4">
+        <f>J20/K20*1000</f>
+        <v>10970268.497189717</v>
+      </c>
+      <c r="M20" s="17">
+        <f>(K16-K20)/K16</f>
+        <v>0.57554069380890926</v>
+      </c>
+      <c r="N20" s="8">
+        <f>(L20-80000000)/80000000</f>
+        <v>-0.86287164378512859</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed castling management fixed promotion management improved calculateCheckPositions
</commit_message>
<xml_diff>
--- a/docs/Performance.xlsx
+++ b/docs/Performance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\clace\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{032B937C-F9BF-412D-AB18-05593EF2EC61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{554C9490-FD93-437A-B42B-D6E1A58EBFD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="5280" windowWidth="29040" windowHeight="15720" xr2:uid="{D3276BA4-EC86-47CC-ADFB-EDF16C1A358E}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>moves</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t>vector pool</t>
+  </si>
+  <si>
+    <t>improved calculateCheckPositions</t>
   </si>
 </sst>
 </file>
@@ -268,7 +271,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -319,6 +322,8 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="10" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -636,10 +641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D63397-ACCF-47C4-BDCB-8082DFD2DBBB}">
-  <dimension ref="A1:P20"/>
+  <dimension ref="A1:P24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1155,19 +1160,19 @@
         <v>206603</v>
       </c>
       <c r="E18" s="20">
-        <v>648</v>
+        <v>641</v>
       </c>
       <c r="F18" s="15">
         <f>D18/E18*1000</f>
-        <v>318831.7901234568</v>
+        <v>322313.57254290173</v>
       </c>
       <c r="G18" s="18">
         <f>(E14-E18)/E14</f>
-        <v>0.16709511568123395</v>
+        <v>0.17609254498714652</v>
       </c>
       <c r="H18" s="16">
         <f>(F18-80000000)/80000000</f>
-        <v>-0.99601460262345676</v>
+        <v>-0.99597108034321369</v>
       </c>
       <c r="I18" s="3">
         <v>4</v>
@@ -1202,19 +1207,19 @@
         <v>5072212</v>
       </c>
       <c r="E19">
-        <v>15906</v>
+        <v>16048</v>
       </c>
       <c r="F19" s="4">
         <f>D19/E19*1000</f>
-        <v>318886.70941782976</v>
+        <v>316065.0548354935</v>
       </c>
       <c r="G19" s="17">
         <f>(E15-E19)/E15</f>
-        <v>0.47388615089471769</v>
+        <v>0.4691892964641286</v>
       </c>
       <c r="H19" s="8">
         <f>(F19-80000000)/80000000</f>
-        <v>-0.99601391613227708</v>
+        <v>-0.99604918681455623</v>
       </c>
       <c r="I19">
         <v>5</v>
@@ -1223,19 +1228,19 @@
         <v>4880523</v>
       </c>
       <c r="K19">
-        <v>441</v>
+        <v>432</v>
       </c>
       <c r="L19" s="4">
         <f>J19/K19*1000</f>
-        <v>11066945.578231292</v>
+        <v>11297506.944444446</v>
       </c>
       <c r="M19" s="17">
         <f>(K15-K19)/K15</f>
-        <v>0.22631578947368422</v>
+        <v>0.24210526315789474</v>
       </c>
       <c r="N19" s="8">
         <f>(L19-80000000)/80000000</f>
-        <v>-0.86166318027210886</v>
+        <v>-0.85878116319444442</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
@@ -1246,19 +1251,137 @@
         <v>119060324</v>
       </c>
       <c r="K20">
-        <v>10853</v>
+        <v>10799</v>
       </c>
       <c r="L20" s="4">
         <f>J20/K20*1000</f>
-        <v>10970268.497189717</v>
+        <v>11025124.918973979</v>
       </c>
       <c r="M20" s="17">
         <f>(K16-K20)/K16</f>
-        <v>0.57554069380890926</v>
+        <v>0.57765262622707181</v>
       </c>
       <c r="N20" s="8">
         <f>(L20-80000000)/80000000</f>
-        <v>-0.86287164378512859</v>
+        <v>-0.86218593851282521</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A22" s="13">
+        <v>45562</v>
+      </c>
+      <c r="B22" s="14"/>
+      <c r="C22" s="19">
+        <v>4</v>
+      </c>
+      <c r="D22" s="15">
+        <v>206603</v>
+      </c>
+      <c r="E22" s="20">
+        <v>595</v>
+      </c>
+      <c r="F22" s="15">
+        <f>D22/E22*1000</f>
+        <v>347231.93277310923</v>
+      </c>
+      <c r="G22" s="18">
+        <f>(E18-E22)/E18</f>
+        <v>7.1762870514820595E-2</v>
+      </c>
+      <c r="H22" s="16">
+        <f>(F22-80000000)/80000000</f>
+        <v>-0.99565960084033611</v>
+      </c>
+      <c r="I22" s="3">
+        <v>4</v>
+      </c>
+      <c r="J22" s="15">
+        <v>197281</v>
+      </c>
+      <c r="K22" s="3">
+        <v>18</v>
+      </c>
+      <c r="L22" s="15">
+        <f>J22/K22*1000</f>
+        <v>10960055.555555554</v>
+      </c>
+      <c r="M22" s="26">
+        <f>(K18-K22)/K18</f>
+        <v>-5.8823529411764705E-2</v>
+      </c>
+      <c r="N22" s="16">
+        <f>(L22-80000000)/80000000</f>
+        <v>-0.8629993055555556</v>
+      </c>
+      <c r="P22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <v>5</v>
+      </c>
+      <c r="D23">
+        <v>5072212</v>
+      </c>
+      <c r="E23">
+        <v>15248</v>
+      </c>
+      <c r="F23" s="4">
+        <f>D23/E23*1000</f>
+        <v>332647.6915005247</v>
+      </c>
+      <c r="G23" s="17">
+        <f>(E19-E23)/E19</f>
+        <v>4.9850448654037885E-2</v>
+      </c>
+      <c r="H23" s="8">
+        <f>(F23-80000000)/80000000</f>
+        <v>-0.99584190385624338</v>
+      </c>
+      <c r="I23">
+        <v>5</v>
+      </c>
+      <c r="J23" s="4">
+        <v>4880523</v>
+      </c>
+      <c r="K23">
+        <v>435</v>
+      </c>
+      <c r="L23" s="4">
+        <f>J23/K23*1000</f>
+        <v>11219593.103448277</v>
+      </c>
+      <c r="M23" s="27">
+        <f>(K19-K23)/K19</f>
+        <v>-6.9444444444444441E-3</v>
+      </c>
+      <c r="N23" s="8">
+        <f>(L23-80000000)/80000000</f>
+        <v>-0.85975508620689656</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I24">
+        <v>6</v>
+      </c>
+      <c r="J24" s="4">
+        <v>119060324</v>
+      </c>
+      <c r="K24">
+        <v>11539</v>
+      </c>
+      <c r="L24" s="4">
+        <f>J24/K24*1000</f>
+        <v>10318079.902937863</v>
+      </c>
+      <c r="M24" s="27">
+        <f>(K20-K24)/K20</f>
+        <v>-6.8524863413279014E-2</v>
+      </c>
+      <c r="N24" s="8">
+        <f>(L24-80000000)/80000000</f>
+        <v>-0.87102400121327672</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added cache for moves generator
</commit_message>
<xml_diff>
--- a/docs/Performance.xlsx
+++ b/docs/Performance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\clace\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{554C9490-FD93-437A-B42B-D6E1A58EBFD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDDA1B45-4ED1-4B41-9BEA-6C91921ECBB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="5280" windowWidth="29040" windowHeight="15720" xr2:uid="{D3276BA4-EC86-47CC-ADFB-EDF16C1A358E}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>moves</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>improved calculateCheckPositions</t>
+  </si>
+  <si>
+    <t>moves cache</t>
   </si>
 </sst>
 </file>
@@ -307,6 +310,8 @@
     <xf numFmtId="10" fontId="5" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -322,8 +327,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -641,10 +644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D63397-ACCF-47C4-BDCB-8082DFD2DBBB}">
-  <dimension ref="A1:P24"/>
+  <dimension ref="A1:P29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -657,22 +660,22 @@
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="10"/>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="24" t="s">
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
       <c r="P1" t="s">
         <v>13</v>
       </c>
@@ -1305,7 +1308,7 @@
         <f>J22/K22*1000</f>
         <v>10960055.555555554</v>
       </c>
-      <c r="M22" s="26">
+      <c r="M22" s="21">
         <f>(K18-K22)/K18</f>
         <v>-5.8823529411764705E-2</v>
       </c>
@@ -1352,7 +1355,7 @@
         <f>J23/K23*1000</f>
         <v>11219593.103448277</v>
       </c>
-      <c r="M23" s="27">
+      <c r="M23" s="22">
         <f>(K19-K23)/K19</f>
         <v>-6.9444444444444441E-3</v>
       </c>
@@ -1375,13 +1378,150 @@
         <f>J24/K24*1000</f>
         <v>10318079.902937863</v>
       </c>
-      <c r="M24" s="27">
+      <c r="M24" s="22">
         <f>(K20-K24)/K20</f>
         <v>-6.8524863413279014E-2</v>
       </c>
       <c r="N24" s="8">
         <f>(L24-80000000)/80000000</f>
         <v>-0.87102400121327672</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A26" s="13">
+        <v>45563</v>
+      </c>
+      <c r="B26" s="14"/>
+      <c r="C26" s="19">
+        <v>4</v>
+      </c>
+      <c r="D26" s="15">
+        <v>206603</v>
+      </c>
+      <c r="E26" s="20">
+        <v>619</v>
+      </c>
+      <c r="F26" s="15">
+        <f>D26/E26*1000</f>
+        <v>333768.98222940223</v>
+      </c>
+      <c r="G26" s="21">
+        <f>(E22-E26)/E22</f>
+        <v>-4.0336134453781515E-2</v>
+      </c>
+      <c r="H26" s="16">
+        <f>(F26-80000000)/80000000</f>
+        <v>-0.99582788772213249</v>
+      </c>
+      <c r="I26" s="3">
+        <v>4</v>
+      </c>
+      <c r="J26" s="15">
+        <v>197281</v>
+      </c>
+      <c r="K26" s="3">
+        <v>25</v>
+      </c>
+      <c r="L26" s="15">
+        <f>J26/K26*1000</f>
+        <v>7891240</v>
+      </c>
+      <c r="M26" s="21">
+        <f>(K22-K26)/K22</f>
+        <v>-0.3888888888888889</v>
+      </c>
+      <c r="N26" s="16">
+        <f>(L26-80000000)/80000000</f>
+        <v>-0.90135949999999998</v>
+      </c>
+      <c r="P26" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <v>5</v>
+      </c>
+      <c r="D27">
+        <v>5072212</v>
+      </c>
+      <c r="E27">
+        <v>11632</v>
+      </c>
+      <c r="F27" s="4">
+        <f>D27/E27*1000</f>
+        <v>436056.74002751033</v>
+      </c>
+      <c r="G27" s="17">
+        <f>(E23-E27)/E23</f>
+        <v>0.23714585519412382</v>
+      </c>
+      <c r="H27" s="8">
+        <f>(F27-80000000)/80000000</f>
+        <v>-0.99454929074965603</v>
+      </c>
+      <c r="I27">
+        <v>5</v>
+      </c>
+      <c r="J27" s="4">
+        <v>4880523</v>
+      </c>
+      <c r="K27">
+        <v>429</v>
+      </c>
+      <c r="L27" s="4">
+        <f>J27/K27*1000</f>
+        <v>11376510.489510488</v>
+      </c>
+      <c r="M27" s="17">
+        <f>(K23-K27)/K23</f>
+        <v>1.3793103448275862E-2</v>
+      </c>
+      <c r="N27" s="8">
+        <f>(L27-80000000)/80000000</f>
+        <v>-0.85779361888111882</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I28">
+        <v>6</v>
+      </c>
+      <c r="J28" s="4">
+        <v>119060324</v>
+      </c>
+      <c r="K28">
+        <v>7892</v>
+      </c>
+      <c r="L28" s="4">
+        <f>J28/K28*1000</f>
+        <v>15086204.257475926</v>
+      </c>
+      <c r="M28" s="17">
+        <f>(K24-K28)/K24</f>
+        <v>0.31605858393274983</v>
+      </c>
+      <c r="N28" s="8">
+        <f>(L28-80000000)/80000000</f>
+        <v>-0.81142244678155095</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I29">
+        <v>7</v>
+      </c>
+      <c r="J29" s="4">
+        <v>3195901860</v>
+      </c>
+      <c r="K29">
+        <v>151609</v>
+      </c>
+      <c r="L29" s="4">
+        <f>J29/K29*1000</f>
+        <v>21079895.38879618</v>
+      </c>
+      <c r="N29" s="22">
+        <f>(L29-80000000)/80000000</f>
+        <v>-0.73650130764004773</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
optimized generation of opposite board
</commit_message>
<xml_diff>
--- a/docs/Performance.xlsx
+++ b/docs/Performance.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t xml:space="preserve">classic</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t xml:space="preserve">linux!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">side</t>
   </si>
   <si>
     <t xml:space="preserve">stockfish livello 1</t>
@@ -291,20 +294,24 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -316,127 +323,131 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="3" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="8" fillId="4" borderId="2" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="3" borderId="3" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="8" fillId="4" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="3" borderId="2" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="3" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="8" fillId="4" borderId="2" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="3" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="8" fillId="4" borderId="2" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="3" borderId="3" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="8" fillId="4" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="3" borderId="2" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="3" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="8" fillId="4" borderId="2" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -692,1028 +703,1146 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P34"/>
+  <dimension ref="A1:P37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H35" activeCellId="0" sqref="H35"/>
+      <selection pane="topLeft" activeCell="H33" activeCellId="0" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="11.57"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="16.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="4.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="4.17"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="4" t="s">
+      <c r="A1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="5" t="s">
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="P1" s="6" t="s">
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="P1" s="7" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="L2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="M2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="8" t="s">
+      <c r="N2" s="9" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="n">
+      <c r="A3" s="10" t="n">
         <v>45404</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="0" t="n">
+      <c r="B3" s="11"/>
+      <c r="C3" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="D3" s="11" t="n">
+      <c r="D3" s="12" t="n">
         <v>206603</v>
       </c>
-      <c r="E3" s="12" t="n">
+      <c r="E3" s="13" t="n">
         <v>1100</v>
       </c>
-      <c r="F3" s="11" t="n">
+      <c r="F3" s="12" t="n">
         <f aca="false">D3/E3*1000</f>
         <v>187820.909090909</v>
       </c>
-      <c r="H3" s="13" t="n">
+      <c r="H3" s="14" t="n">
         <f aca="false">(F3-80000000)/80000000</f>
         <v>-0.997652238636364</v>
       </c>
-      <c r="I3" s="0" t="n">
+      <c r="I3" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="J3" s="11" t="n">
+      <c r="J3" s="12" t="n">
         <v>197281</v>
       </c>
-      <c r="K3" s="0" t="n">
+      <c r="K3" s="2" t="n">
         <v>62</v>
       </c>
-      <c r="L3" s="11" t="n">
+      <c r="L3" s="12" t="n">
         <f aca="false">J3/K3*1000</f>
         <v>3181951.61290323</v>
       </c>
-      <c r="N3" s="13" t="n">
+      <c r="N3" s="14" t="n">
         <f aca="false">(L3-80000000)/80000000</f>
         <v>-0.96022560483871</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="14"/>
-      <c r="C4" s="0" t="n">
+      <c r="B4" s="15"/>
+      <c r="C4" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="2" t="n">
         <v>5072212</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="2" t="n">
         <v>42000</v>
       </c>
-      <c r="F4" s="11" t="n">
+      <c r="F4" s="12" t="n">
         <f aca="false">D4/E4*1000</f>
         <v>120766.952380952</v>
       </c>
-      <c r="H4" s="13" t="n">
+      <c r="H4" s="14" t="n">
         <f aca="false">(F4-80000000)/80000000</f>
         <v>-0.998490413095238</v>
       </c>
-      <c r="I4" s="0" t="n">
+      <c r="I4" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="J4" s="11" t="n">
+      <c r="J4" s="12" t="n">
         <v>4880523</v>
       </c>
-      <c r="K4" s="0" t="n">
+      <c r="K4" s="2" t="n">
         <v>945</v>
       </c>
-      <c r="L4" s="11" t="n">
+      <c r="L4" s="12" t="n">
         <f aca="false">J4/K4*1000</f>
         <v>5164574.6031746</v>
       </c>
-      <c r="N4" s="13" t="n">
+      <c r="N4" s="14" t="n">
         <f aca="false">(L4-80000000)/80000000</f>
         <v>-0.935442817460318</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="15" t="n">
+      <c r="A6" s="16" t="n">
         <v>45553</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="17" t="n">
+      <c r="B6" s="17"/>
+      <c r="C6" s="18" t="n">
         <v>4</v>
       </c>
-      <c r="D6" s="18" t="n">
+      <c r="D6" s="19" t="n">
         <v>206603</v>
       </c>
-      <c r="E6" s="19" t="n">
+      <c r="E6" s="20" t="n">
         <v>909</v>
       </c>
-      <c r="F6" s="18" t="n">
+      <c r="F6" s="19" t="n">
         <f aca="false">D6/E6*1000</f>
         <v>227286.02860286</v>
       </c>
-      <c r="G6" s="20" t="n">
+      <c r="G6" s="21" t="n">
         <f aca="false">(E3-E6)/E3</f>
         <v>0.173636363636364</v>
       </c>
-      <c r="H6" s="21" t="n">
+      <c r="H6" s="22" t="n">
         <f aca="false">(F6-80000000)/80000000</f>
         <v>-0.997158924642464</v>
       </c>
-      <c r="I6" s="2" t="n">
+      <c r="I6" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="J6" s="18" t="n">
+      <c r="J6" s="19" t="n">
         <v>197281</v>
       </c>
-      <c r="K6" s="2" t="n">
+      <c r="K6" s="3" t="n">
         <v>48</v>
       </c>
-      <c r="L6" s="18" t="n">
+      <c r="L6" s="19" t="n">
         <f aca="false">J6/K6*1000</f>
         <v>4110020.83333333</v>
       </c>
-      <c r="M6" s="20" t="n">
+      <c r="M6" s="21" t="n">
         <f aca="false">(K3-K6)/K3</f>
         <v>0.225806451612903</v>
       </c>
-      <c r="N6" s="21" t="n">
+      <c r="N6" s="22" t="n">
         <f aca="false">(L6-80000000)/80000000</f>
         <v>-0.948624739583333</v>
       </c>
-      <c r="P6" s="6" t="s">
+      <c r="P6" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="2" t="n">
         <v>5072212</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7" s="2" t="n">
         <v>34300</v>
       </c>
-      <c r="F7" s="11" t="n">
+      <c r="F7" s="12" t="n">
         <f aca="false">D7/E7*1000</f>
         <v>147877.900874636</v>
       </c>
-      <c r="G7" s="22" t="n">
+      <c r="G7" s="23" t="n">
         <f aca="false">(E4-E7)/E4</f>
         <v>0.183333333333333</v>
       </c>
-      <c r="H7" s="13" t="n">
+      <c r="H7" s="14" t="n">
         <f aca="false">(F7-80000000)/80000000</f>
         <v>-0.998151526239067</v>
       </c>
-      <c r="I7" s="0" t="n">
+      <c r="I7" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="J7" s="11" t="n">
+      <c r="J7" s="12" t="n">
         <v>4880523</v>
       </c>
-      <c r="K7" s="0" t="n">
+      <c r="K7" s="2" t="n">
         <v>727</v>
       </c>
-      <c r="L7" s="11" t="n">
+      <c r="L7" s="12" t="n">
         <f aca="false">J7/K7*1000</f>
         <v>6713236.58872077</v>
       </c>
-      <c r="M7" s="22" t="n">
+      <c r="M7" s="23" t="n">
         <f aca="false">(K4-K7)/K4</f>
         <v>0.230687830687831</v>
       </c>
-      <c r="N7" s="13" t="n">
+      <c r="N7" s="14" t="n">
         <f aca="false">(L7-80000000)/80000000</f>
         <v>-0.91608454264099</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I8" s="0" t="n">
+      <c r="I8" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="J8" s="11" t="n">
+      <c r="J8" s="12" t="n">
         <v>119060324</v>
       </c>
-      <c r="K8" s="0" t="n">
+      <c r="K8" s="2" t="n">
         <v>29235</v>
       </c>
-      <c r="L8" s="11" t="n">
+      <c r="L8" s="12" t="n">
         <f aca="false">J8/K8*1000</f>
         <v>4072526.90268514</v>
       </c>
-      <c r="N8" s="13" t="n">
+      <c r="N8" s="14" t="n">
         <f aca="false">(L8-80000000)/80000000</f>
         <v>-0.949093413716436</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="15" t="n">
+      <c r="A10" s="16" t="n">
         <v>45554</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="17" t="n">
+      <c r="B10" s="17"/>
+      <c r="C10" s="18" t="n">
         <v>4</v>
       </c>
-      <c r="D10" s="18" t="n">
+      <c r="D10" s="19" t="n">
         <v>206603</v>
       </c>
-      <c r="E10" s="19" t="n">
+      <c r="E10" s="20" t="n">
         <v>822</v>
       </c>
-      <c r="F10" s="18" t="n">
+      <c r="F10" s="19" t="n">
         <f aca="false">D10/E10*1000</f>
         <v>251341.849148419</v>
       </c>
-      <c r="G10" s="20" t="n">
+      <c r="G10" s="21" t="n">
         <f aca="false">(E6-E10)/E6</f>
         <v>0.0957095709570957</v>
       </c>
-      <c r="H10" s="21" t="n">
+      <c r="H10" s="22" t="n">
         <f aca="false">(F10-80000000)/80000000</f>
         <v>-0.996858226885645</v>
       </c>
-      <c r="I10" s="2" t="n">
+      <c r="I10" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="J10" s="18" t="n">
+      <c r="J10" s="19" t="n">
         <v>197281</v>
       </c>
-      <c r="K10" s="2" t="n">
+      <c r="K10" s="3" t="n">
         <v>42</v>
       </c>
-      <c r="L10" s="18" t="n">
+      <c r="L10" s="19" t="n">
         <f aca="false">J10/K10*1000</f>
         <v>4697166.66666667</v>
       </c>
-      <c r="M10" s="20" t="n">
+      <c r="M10" s="21" t="n">
         <f aca="false">(K6-K10)/K6</f>
         <v>0.125</v>
       </c>
-      <c r="N10" s="21" t="n">
+      <c r="N10" s="22" t="n">
         <f aca="false">(L10-80000000)/80000000</f>
         <v>-0.941285416666667</v>
       </c>
-      <c r="P10" s="6" t="s">
+      <c r="P10" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="0" t="n">
+      <c r="C11" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="D11" s="2" t="n">
         <v>5072212</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="E11" s="2" t="n">
         <v>30566</v>
       </c>
-      <c r="F11" s="11" t="n">
+      <c r="F11" s="12" t="n">
         <f aca="false">D11/E11*1000</f>
         <v>165942.943139436</v>
       </c>
-      <c r="G11" s="22" t="n">
+      <c r="G11" s="23" t="n">
         <f aca="false">(E7-E11)/E7</f>
         <v>0.108862973760933</v>
       </c>
-      <c r="H11" s="13" t="n">
+      <c r="H11" s="14" t="n">
         <f aca="false">(F11-80000000)/80000000</f>
         <v>-0.997925713210757</v>
       </c>
-      <c r="I11" s="0" t="n">
+      <c r="I11" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="J11" s="11" t="n">
+      <c r="J11" s="12" t="n">
         <v>4880523</v>
       </c>
-      <c r="K11" s="0" t="n">
+      <c r="K11" s="2" t="n">
         <v>631</v>
       </c>
-      <c r="L11" s="11" t="n">
+      <c r="L11" s="12" t="n">
         <f aca="false">J11/K11*1000</f>
         <v>7734584.78605388</v>
       </c>
-      <c r="M11" s="22" t="n">
+      <c r="M11" s="23" t="n">
         <f aca="false">(K7-K11)/K7</f>
         <v>0.132049518569464</v>
       </c>
-      <c r="N11" s="13" t="n">
+      <c r="N11" s="14" t="n">
         <f aca="false">(L11-80000000)/80000000</f>
         <v>-0.903317690174327</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I12" s="0" t="n">
+      <c r="I12" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="J12" s="11" t="n">
+      <c r="J12" s="12" t="n">
         <v>119060324</v>
       </c>
-      <c r="K12" s="0" t="n">
+      <c r="K12" s="2" t="n">
         <v>25861</v>
       </c>
-      <c r="L12" s="11" t="n">
+      <c r="L12" s="12" t="n">
         <f aca="false">J12/K12*1000</f>
         <v>4603856.15405437</v>
       </c>
-      <c r="M12" s="22" t="n">
+      <c r="M12" s="23" t="n">
         <f aca="false">(K8-K12)/K8</f>
         <v>0.115409611766718</v>
       </c>
-      <c r="N12" s="13" t="n">
+      <c r="N12" s="14" t="n">
         <f aca="false">(L12-80000000)/80000000</f>
         <v>-0.94245179807432</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="15" t="n">
+      <c r="A14" s="16" t="n">
         <v>45557</v>
       </c>
-      <c r="B14" s="16"/>
-      <c r="C14" s="17" t="n">
+      <c r="B14" s="17"/>
+      <c r="C14" s="18" t="n">
         <v>4</v>
       </c>
-      <c r="D14" s="18" t="n">
+      <c r="D14" s="19" t="n">
         <v>206603</v>
       </c>
-      <c r="E14" s="19" t="n">
+      <c r="E14" s="20" t="n">
         <v>778</v>
       </c>
-      <c r="F14" s="18" t="n">
+      <c r="F14" s="19" t="n">
         <f aca="false">D14/E14*1000</f>
         <v>265556.555269923</v>
       </c>
-      <c r="G14" s="20" t="n">
+      <c r="G14" s="21" t="n">
         <f aca="false">(E10-E14)/E10</f>
         <v>0.0535279805352798</v>
       </c>
-      <c r="H14" s="21" t="n">
+      <c r="H14" s="22" t="n">
         <f aca="false">(F14-80000000)/80000000</f>
         <v>-0.996680543059126</v>
       </c>
-      <c r="I14" s="2" t="n">
+      <c r="I14" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="J14" s="18" t="n">
+      <c r="J14" s="19" t="n">
         <v>197281</v>
       </c>
-      <c r="K14" s="2" t="n">
+      <c r="K14" s="3" t="n">
         <v>42</v>
       </c>
-      <c r="L14" s="18" t="n">
+      <c r="L14" s="19" t="n">
         <f aca="false">J14/K14*1000</f>
         <v>4697166.66666667</v>
       </c>
-      <c r="M14" s="20" t="n">
+      <c r="M14" s="21" t="n">
         <f aca="false">(K10-K14)/K10</f>
         <v>0</v>
       </c>
-      <c r="N14" s="21" t="n">
+      <c r="N14" s="22" t="n">
         <f aca="false">(L14-80000000)/80000000</f>
         <v>-0.941285416666667</v>
       </c>
-      <c r="P14" s="6" t="s">
+      <c r="P14" s="7" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C15" s="0" t="n">
+      <c r="C15" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="D15" s="2" t="n">
         <v>5072212</v>
       </c>
-      <c r="E15" s="0" t="n">
+      <c r="E15" s="2" t="n">
         <v>30233</v>
       </c>
-      <c r="F15" s="11" t="n">
+      <c r="F15" s="12" t="n">
         <f aca="false">D15/E15*1000</f>
         <v>167770.714120332</v>
       </c>
-      <c r="G15" s="22" t="n">
+      <c r="G15" s="23" t="n">
         <f aca="false">(E11-E15)/E11</f>
         <v>0.0108944578943925</v>
       </c>
-      <c r="H15" s="13" t="n">
+      <c r="H15" s="14" t="n">
         <f aca="false">(F15-80000000)/80000000</f>
         <v>-0.997902866073496</v>
       </c>
-      <c r="I15" s="0" t="n">
+      <c r="I15" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="J15" s="11" t="n">
+      <c r="J15" s="12" t="n">
         <v>4880523</v>
       </c>
-      <c r="K15" s="0" t="n">
+      <c r="K15" s="2" t="n">
         <v>570</v>
       </c>
-      <c r="L15" s="11" t="n">
+      <c r="L15" s="12" t="n">
         <f aca="false">J15/K15*1000</f>
         <v>8562321.05263158</v>
       </c>
-      <c r="M15" s="22" t="n">
+      <c r="M15" s="23" t="n">
         <f aca="false">(K11-K15)/K11</f>
         <v>0.0966719492868463</v>
       </c>
-      <c r="N15" s="13" t="n">
+      <c r="N15" s="14" t="n">
         <f aca="false">(L15-80000000)/80000000</f>
         <v>-0.892970986842105</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I16" s="0" t="n">
+      <c r="I16" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="J16" s="11" t="n">
+      <c r="J16" s="12" t="n">
         <v>119060324</v>
       </c>
-      <c r="K16" s="0" t="n">
+      <c r="K16" s="2" t="n">
         <v>25569</v>
       </c>
-      <c r="L16" s="11" t="n">
+      <c r="L16" s="12" t="n">
         <f aca="false">J16/K16*1000</f>
         <v>4656432.55504713</v>
       </c>
-      <c r="M16" s="22" t="n">
+      <c r="M16" s="23" t="n">
         <f aca="false">(K12-K16)/K12</f>
         <v>0.0112911333668458</v>
       </c>
-      <c r="N16" s="13" t="n">
+      <c r="N16" s="14" t="n">
         <f aca="false">(L16-80000000)/80000000</f>
         <v>-0.941794593061911</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="15" t="n">
+      <c r="A18" s="16" t="n">
         <v>45559</v>
       </c>
-      <c r="B18" s="16"/>
-      <c r="C18" s="17" t="n">
+      <c r="B18" s="17"/>
+      <c r="C18" s="18" t="n">
         <v>4</v>
       </c>
-      <c r="D18" s="18" t="n">
+      <c r="D18" s="19" t="n">
         <v>206603</v>
       </c>
-      <c r="E18" s="19" t="n">
+      <c r="E18" s="20" t="n">
         <v>641</v>
       </c>
-      <c r="F18" s="18" t="n">
+      <c r="F18" s="19" t="n">
         <f aca="false">D18/E18*1000</f>
         <v>322313.572542902</v>
       </c>
-      <c r="G18" s="20" t="n">
+      <c r="G18" s="21" t="n">
         <f aca="false">(E14-E18)/E14</f>
         <v>0.176092544987147</v>
       </c>
-      <c r="H18" s="21" t="n">
+      <c r="H18" s="22" t="n">
         <f aca="false">(F18-80000000)/80000000</f>
         <v>-0.995971080343214</v>
       </c>
-      <c r="I18" s="2" t="n">
+      <c r="I18" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="J18" s="18" t="n">
+      <c r="J18" s="19" t="n">
         <v>197281</v>
       </c>
-      <c r="K18" s="2" t="n">
+      <c r="K18" s="3" t="n">
         <v>17</v>
       </c>
-      <c r="L18" s="18" t="n">
+      <c r="L18" s="19" t="n">
         <f aca="false">J18/K18*1000</f>
         <v>11604764.7058824</v>
       </c>
-      <c r="M18" s="20" t="n">
+      <c r="M18" s="21" t="n">
         <f aca="false">(K14-K18)/K14</f>
         <v>0.595238095238095</v>
       </c>
-      <c r="N18" s="21" t="n">
+      <c r="N18" s="22" t="n">
         <f aca="false">(L18-80000000)/80000000</f>
         <v>-0.854940441176471</v>
       </c>
-      <c r="P18" s="6" t="s">
+      <c r="P18" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="0" t="n">
+      <c r="C19" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="D19" s="0" t="n">
+      <c r="D19" s="2" t="n">
         <v>5072212</v>
       </c>
-      <c r="E19" s="0" t="n">
+      <c r="E19" s="2" t="n">
         <v>16048</v>
       </c>
-      <c r="F19" s="11" t="n">
+      <c r="F19" s="12" t="n">
         <f aca="false">D19/E19*1000</f>
         <v>316065.054835494</v>
       </c>
-      <c r="G19" s="22" t="n">
+      <c r="G19" s="23" t="n">
         <f aca="false">(E15-E19)/E15</f>
         <v>0.469189296464129</v>
       </c>
-      <c r="H19" s="13" t="n">
+      <c r="H19" s="14" t="n">
         <f aca="false">(F19-80000000)/80000000</f>
         <v>-0.996049186814556</v>
       </c>
-      <c r="I19" s="0" t="n">
+      <c r="I19" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="J19" s="11" t="n">
+      <c r="J19" s="12" t="n">
         <v>4880523</v>
       </c>
-      <c r="K19" s="0" t="n">
+      <c r="K19" s="2" t="n">
         <v>432</v>
       </c>
-      <c r="L19" s="11" t="n">
+      <c r="L19" s="12" t="n">
         <f aca="false">J19/K19*1000</f>
         <v>11297506.9444444</v>
       </c>
-      <c r="M19" s="22" t="n">
+      <c r="M19" s="23" t="n">
         <f aca="false">(K15-K19)/K15</f>
         <v>0.242105263157895</v>
       </c>
-      <c r="N19" s="13" t="n">
+      <c r="N19" s="14" t="n">
         <f aca="false">(L19-80000000)/80000000</f>
         <v>-0.858781163194444</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I20" s="0" t="n">
+      <c r="I20" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="J20" s="11" t="n">
+      <c r="J20" s="12" t="n">
         <v>119060324</v>
       </c>
-      <c r="K20" s="0" t="n">
+      <c r="K20" s="2" t="n">
         <v>10799</v>
       </c>
-      <c r="L20" s="11" t="n">
+      <c r="L20" s="12" t="n">
         <f aca="false">J20/K20*1000</f>
         <v>11025124.918974</v>
       </c>
-      <c r="M20" s="22" t="n">
+      <c r="M20" s="23" t="n">
         <f aca="false">(K16-K20)/K16</f>
         <v>0.577652626227072</v>
       </c>
-      <c r="N20" s="13" t="n">
+      <c r="N20" s="14" t="n">
         <f aca="false">(L20-80000000)/80000000</f>
         <v>-0.862185938512825</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="15" t="n">
+      <c r="A22" s="16" t="n">
         <v>45562</v>
       </c>
-      <c r="B22" s="16"/>
-      <c r="C22" s="17" t="n">
+      <c r="B22" s="17"/>
+      <c r="C22" s="18" t="n">
         <v>4</v>
       </c>
-      <c r="D22" s="18" t="n">
+      <c r="D22" s="19" t="n">
         <v>206603</v>
       </c>
-      <c r="E22" s="19" t="n">
+      <c r="E22" s="20" t="n">
         <v>595</v>
       </c>
-      <c r="F22" s="18" t="n">
+      <c r="F22" s="19" t="n">
         <f aca="false">D22/E22*1000</f>
         <v>347231.932773109</v>
       </c>
-      <c r="G22" s="20" t="n">
+      <c r="G22" s="21" t="n">
         <f aca="false">(E18-E22)/E18</f>
         <v>0.0717628705148206</v>
       </c>
-      <c r="H22" s="21" t="n">
+      <c r="H22" s="22" t="n">
         <f aca="false">(F22-80000000)/80000000</f>
         <v>-0.995659600840336</v>
       </c>
-      <c r="I22" s="2" t="n">
+      <c r="I22" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="J22" s="18" t="n">
+      <c r="J22" s="19" t="n">
         <v>197281</v>
       </c>
-      <c r="K22" s="2" t="n">
+      <c r="K22" s="3" t="n">
         <v>18</v>
       </c>
-      <c r="L22" s="18" t="n">
+      <c r="L22" s="19" t="n">
         <f aca="false">J22/K22*1000</f>
         <v>10960055.5555556</v>
       </c>
-      <c r="M22" s="23" t="n">
+      <c r="M22" s="24" t="n">
         <f aca="false">(K18-K22)/K18</f>
         <v>-0.0588235294117647</v>
       </c>
-      <c r="N22" s="21" t="n">
+      <c r="N22" s="22" t="n">
         <f aca="false">(L22-80000000)/80000000</f>
         <v>-0.862999305555556</v>
       </c>
-      <c r="P22" s="6" t="s">
+      <c r="P22" s="7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C23" s="0" t="n">
+      <c r="C23" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="D23" s="0" t="n">
+      <c r="D23" s="2" t="n">
         <v>5072212</v>
       </c>
-      <c r="E23" s="0" t="n">
+      <c r="E23" s="2" t="n">
         <v>15248</v>
       </c>
-      <c r="F23" s="11" t="n">
+      <c r="F23" s="12" t="n">
         <f aca="false">D23/E23*1000</f>
         <v>332647.691500525</v>
       </c>
-      <c r="G23" s="22" t="n">
+      <c r="G23" s="23" t="n">
         <f aca="false">(E19-E23)/E19</f>
         <v>0.0498504486540379</v>
       </c>
-      <c r="H23" s="13" t="n">
+      <c r="H23" s="14" t="n">
         <f aca="false">(F23-80000000)/80000000</f>
         <v>-0.995841903856243</v>
       </c>
-      <c r="I23" s="0" t="n">
+      <c r="I23" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="J23" s="11" t="n">
+      <c r="J23" s="12" t="n">
         <v>4880523</v>
       </c>
-      <c r="K23" s="0" t="n">
+      <c r="K23" s="2" t="n">
         <v>435</v>
       </c>
-      <c r="L23" s="11" t="n">
+      <c r="L23" s="12" t="n">
         <f aca="false">J23/K23*1000</f>
         <v>11219593.1034483</v>
       </c>
-      <c r="M23" s="24" t="n">
+      <c r="M23" s="25" t="n">
         <f aca="false">(K19-K23)/K19</f>
         <v>-0.00694444444444444</v>
       </c>
-      <c r="N23" s="13" t="n">
+      <c r="N23" s="14" t="n">
         <f aca="false">(L23-80000000)/80000000</f>
         <v>-0.859755086206897</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I24" s="0" t="n">
+      <c r="I24" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="J24" s="11" t="n">
+      <c r="J24" s="12" t="n">
         <v>119060324</v>
       </c>
-      <c r="K24" s="0" t="n">
+      <c r="K24" s="2" t="n">
         <v>11539</v>
       </c>
-      <c r="L24" s="11" t="n">
+      <c r="L24" s="12" t="n">
         <f aca="false">J24/K24*1000</f>
         <v>10318079.9029379</v>
       </c>
-      <c r="M24" s="24" t="n">
+      <c r="M24" s="25" t="n">
         <f aca="false">(K20-K24)/K20</f>
         <v>-0.068524863413279</v>
       </c>
-      <c r="N24" s="13" t="n">
+      <c r="N24" s="14" t="n">
         <f aca="false">(L24-80000000)/80000000</f>
         <v>-0.871024001213277</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="25" t="n">
+      <c r="A26" s="26" t="n">
         <v>45563</v>
       </c>
-      <c r="B26" s="26"/>
-      <c r="C26" s="27" t="n">
+      <c r="B26" s="27"/>
+      <c r="C26" s="28" t="n">
         <v>4</v>
       </c>
-      <c r="D26" s="28" t="n">
+      <c r="D26" s="29" t="n">
         <v>206603</v>
       </c>
-      <c r="E26" s="29" t="n">
+      <c r="E26" s="30" t="n">
         <v>619</v>
       </c>
-      <c r="F26" s="28" t="n">
+      <c r="F26" s="29" t="n">
         <f aca="false">D26/E26*1000</f>
         <v>333768.982229402</v>
       </c>
-      <c r="G26" s="23" t="n">
+      <c r="G26" s="24" t="n">
         <f aca="false">(E22-E26)/E22</f>
         <v>-0.0403361344537815</v>
       </c>
-      <c r="H26" s="21" t="n">
+      <c r="H26" s="22" t="n">
         <f aca="false">(F26-80000000)/80000000</f>
         <v>-0.995827887722133</v>
       </c>
-      <c r="I26" s="30" t="n">
+      <c r="I26" s="31" t="n">
         <v>4</v>
       </c>
-      <c r="J26" s="28" t="n">
+      <c r="J26" s="29" t="n">
         <v>197281</v>
       </c>
-      <c r="K26" s="30" t="n">
+      <c r="K26" s="31" t="n">
         <v>25</v>
       </c>
-      <c r="L26" s="28" t="n">
+      <c r="L26" s="29" t="n">
         <f aca="false">J26/K26*1000</f>
         <v>7891240</v>
       </c>
-      <c r="M26" s="23" t="n">
+      <c r="M26" s="24" t="n">
         <f aca="false">(K22-K26)/K22</f>
         <v>-0.388888888888889</v>
       </c>
-      <c r="N26" s="21" t="n">
+      <c r="N26" s="22" t="n">
         <f aca="false">(L26-80000000)/80000000</f>
         <v>-0.9013595</v>
       </c>
-      <c r="P26" s="31" t="s">
+      <c r="P26" s="32" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="31"/>
-      <c r="B27" s="32"/>
-      <c r="C27" s="31" t="n">
+      <c r="A27" s="32"/>
+      <c r="B27" s="33"/>
+      <c r="C27" s="32" t="n">
         <v>5</v>
       </c>
-      <c r="D27" s="31" t="n">
+      <c r="D27" s="32" t="n">
         <v>5072212</v>
       </c>
-      <c r="E27" s="31" t="n">
+      <c r="E27" s="32" t="n">
         <v>11632</v>
       </c>
-      <c r="F27" s="33" t="n">
+      <c r="F27" s="34" t="n">
         <f aca="false">D27/E27*1000</f>
         <v>436056.74002751</v>
       </c>
-      <c r="G27" s="22" t="n">
+      <c r="G27" s="23" t="n">
         <f aca="false">(E23-E27)/E23</f>
         <v>0.237145855194124</v>
       </c>
-      <c r="H27" s="13" t="n">
+      <c r="H27" s="14" t="n">
         <f aca="false">(F27-80000000)/80000000</f>
         <v>-0.994549290749656</v>
       </c>
-      <c r="I27" s="31" t="n">
+      <c r="I27" s="32" t="n">
         <v>5</v>
       </c>
-      <c r="J27" s="33" t="n">
+      <c r="J27" s="34" t="n">
         <v>4880523</v>
       </c>
-      <c r="K27" s="31" t="n">
+      <c r="K27" s="32" t="n">
         <v>429</v>
       </c>
-      <c r="L27" s="33" t="n">
+      <c r="L27" s="34" t="n">
         <f aca="false">J27/K27*1000</f>
         <v>11376510.4895105</v>
       </c>
-      <c r="M27" s="22" t="n">
+      <c r="M27" s="23" t="n">
         <f aca="false">(K23-K27)/K23</f>
         <v>0.0137931034482759</v>
       </c>
-      <c r="N27" s="13" t="n">
+      <c r="N27" s="14" t="n">
         <f aca="false">(L27-80000000)/80000000</f>
         <v>-0.857793618881119</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="31"/>
-      <c r="B28" s="32"/>
-      <c r="C28" s="31"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="31" t="n">
+      <c r="A28" s="32"/>
+      <c r="B28" s="33"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="33"/>
+      <c r="I28" s="32" t="n">
         <v>6</v>
       </c>
-      <c r="J28" s="33" t="n">
+      <c r="J28" s="34" t="n">
         <v>119060324</v>
       </c>
-      <c r="K28" s="31" t="n">
+      <c r="K28" s="32" t="n">
         <v>7892</v>
       </c>
-      <c r="L28" s="33" t="n">
+      <c r="L28" s="34" t="n">
         <f aca="false">J28/K28*1000</f>
         <v>15086204.2574759</v>
       </c>
-      <c r="M28" s="22" t="n">
+      <c r="M28" s="23" t="n">
         <f aca="false">(K24-K28)/K24</f>
         <v>0.31605858393275</v>
       </c>
-      <c r="N28" s="13" t="n">
+      <c r="N28" s="14" t="n">
         <f aca="false">(L28-80000000)/80000000</f>
         <v>-0.811422446781551</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="31"/>
-      <c r="B29" s="32"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="32"/>
-      <c r="I29" s="31" t="n">
+      <c r="A29" s="32"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="33"/>
+      <c r="I29" s="32" t="n">
         <v>7</v>
       </c>
-      <c r="J29" s="33" t="n">
+      <c r="J29" s="34" t="n">
         <v>3195901860</v>
       </c>
-      <c r="K29" s="31" t="n">
+      <c r="K29" s="32" t="n">
         <v>151609</v>
       </c>
-      <c r="L29" s="33" t="n">
+      <c r="L29" s="34" t="n">
         <f aca="false">J29/K29*1000</f>
         <v>21079895.3887962</v>
       </c>
-      <c r="M29" s="31"/>
-      <c r="N29" s="24" t="n">
+      <c r="M29" s="32"/>
+      <c r="N29" s="25" t="n">
         <f aca="false">(L29-80000000)/80000000</f>
         <v>-0.736501307640048</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="15" t="n">
+      <c r="A31" s="16" t="n">
         <v>45568</v>
       </c>
-      <c r="B31" s="16"/>
-      <c r="C31" s="17" t="n">
+      <c r="B31" s="17"/>
+      <c r="C31" s="18" t="n">
         <v>4</v>
       </c>
-      <c r="D31" s="18" t="n">
+      <c r="D31" s="19" t="n">
         <v>206603</v>
       </c>
-      <c r="E31" s="19" t="n">
+      <c r="E31" s="20" t="n">
         <v>559</v>
       </c>
-      <c r="F31" s="18" t="n">
+      <c r="F31" s="19" t="n">
         <f aca="false">D31/E31*1000</f>
         <v>369593.917710197</v>
       </c>
-      <c r="G31" s="34" t="n">
+      <c r="G31" s="35" t="n">
         <f aca="false">(E22-E31)/E22</f>
         <v>0.0605042016806723</v>
       </c>
-      <c r="H31" s="21" t="n">
+      <c r="H31" s="22" t="n">
         <f aca="false">(F31-80000000)/80000000</f>
         <v>-0.995380076028623</v>
       </c>
-      <c r="I31" s="2" t="n">
+      <c r="I31" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="J31" s="18" t="n">
+      <c r="J31" s="19" t="n">
         <v>197281</v>
       </c>
-      <c r="K31" s="2" t="n">
+      <c r="K31" s="3" t="n">
         <v>18</v>
       </c>
-      <c r="L31" s="18" t="n">
+      <c r="L31" s="19" t="n">
         <f aca="false">J31/K31*1000</f>
         <v>10960055.5555556</v>
       </c>
-      <c r="M31" s="23" t="n">
+      <c r="M31" s="24" t="n">
         <f aca="false">(K22-K31)/K22</f>
         <v>0</v>
       </c>
-      <c r="N31" s="21" t="n">
+      <c r="N31" s="22" t="n">
         <f aca="false">(L31-80000000)/80000000</f>
         <v>-0.862999305555556</v>
       </c>
-      <c r="P31" s="6" t="s">
+      <c r="P31" s="7" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C32" s="0" t="n">
+      <c r="C32" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="D32" s="0" t="n">
+      <c r="D32" s="2" t="n">
         <v>5072212</v>
       </c>
-      <c r="E32" s="0" t="n">
+      <c r="E32" s="2" t="n">
         <v>15191</v>
       </c>
-      <c r="F32" s="11" t="n">
+      <c r="F32" s="12" t="n">
         <f aca="false">D32/E32*1000</f>
         <v>333895.859390429</v>
       </c>
-      <c r="G32" s="22" t="n">
+      <c r="G32" s="23" t="n">
         <f aca="false">(E23-E32)/E23</f>
         <v>0.00373819517313746</v>
       </c>
-      <c r="H32" s="13" t="n">
+      <c r="H32" s="14" t="n">
         <f aca="false">(F32-80000000)/80000000</f>
         <v>-0.99582630175762</v>
       </c>
-      <c r="I32" s="0" t="n">
+      <c r="I32" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="J32" s="11" t="n">
+      <c r="J32" s="12" t="n">
         <v>4880523</v>
       </c>
-      <c r="K32" s="0" t="n">
+      <c r="K32" s="2" t="n">
         <v>410</v>
       </c>
-      <c r="L32" s="11" t="n">
+      <c r="L32" s="12" t="n">
         <f aca="false">J32/K32*1000</f>
         <v>11903714.6341463</v>
       </c>
-      <c r="M32" s="22" t="n">
+      <c r="M32" s="23" t="n">
         <f aca="false">(K23-K32)/K23</f>
         <v>0.0574712643678161</v>
       </c>
-      <c r="N32" s="13" t="n">
+      <c r="N32" s="14" t="n">
         <f aca="false">(L32-80000000)/80000000</f>
         <v>-0.851203567073171</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I33" s="0" t="n">
+      <c r="I33" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="J33" s="11" t="n">
+      <c r="J33" s="12" t="n">
         <v>119060324</v>
       </c>
-      <c r="K33" s="0" t="n">
+      <c r="K33" s="2" t="n">
         <v>11511</v>
       </c>
-      <c r="L33" s="11" t="n">
+      <c r="L33" s="12" t="n">
         <f aca="false">J33/K33*1000</f>
         <v>10343178.1773955</v>
       </c>
-      <c r="M33" s="22" t="n">
+      <c r="M33" s="23" t="n">
         <f aca="false">(K24-K33)/K24</f>
         <v>0.00242655342750672</v>
       </c>
-      <c r="N33" s="13" t="n">
+      <c r="N33" s="14" t="n">
         <f aca="false">(L33-80000000)/80000000</f>
         <v>-0.870710272782556</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J34" s="11"/>
-      <c r="L34" s="11"/>
-      <c r="N34" s="35"/>
+      <c r="J34" s="12"/>
+      <c r="L34" s="12"/>
+      <c r="N34" s="36"/>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="16" t="n">
+        <v>45569</v>
+      </c>
+      <c r="B35" s="17"/>
+      <c r="C35" s="18" t="n">
+        <v>4</v>
+      </c>
+      <c r="D35" s="19" t="n">
+        <v>206603</v>
+      </c>
+      <c r="E35" s="20" t="n">
+        <v>607</v>
+      </c>
+      <c r="F35" s="19" t="n">
+        <f aca="false">D35/E35*1000</f>
+        <v>340367.380560132</v>
+      </c>
+      <c r="G35" s="22" t="n">
+        <f aca="false">(E31-E35)/E31</f>
+        <v>-0.0858676207513417</v>
+      </c>
+      <c r="H35" s="22" t="n">
+        <f aca="false">(F35-80000000)/80000000</f>
+        <v>-0.995745407742998</v>
+      </c>
+      <c r="I35" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="J35" s="19" t="n">
+        <v>197281</v>
+      </c>
+      <c r="K35" s="3" t="n">
+        <v>18</v>
+      </c>
+      <c r="L35" s="19" t="n">
+        <f aca="false">J35/K35*1000</f>
+        <v>10960055.5555556</v>
+      </c>
+      <c r="M35" s="24" t="n">
+        <f aca="false">(K31-K35)/K31</f>
+        <v>0</v>
+      </c>
+      <c r="N35" s="22" t="n">
+        <f aca="false">(L35-80000000)/80000000</f>
+        <v>-0.862999305555556</v>
+      </c>
+      <c r="P35" s="37" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C36" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="D36" s="2" t="n">
+        <v>5072212</v>
+      </c>
+      <c r="E36" s="2" t="n">
+        <v>15083</v>
+      </c>
+      <c r="F36" s="12" t="n">
+        <f aca="false">D36/E36*1000</f>
+        <v>336286.680368627</v>
+      </c>
+      <c r="G36" s="23" t="n">
+        <f aca="false">(E32-E36)/E32</f>
+        <v>0.00710947271410704</v>
+      </c>
+      <c r="H36" s="14" t="n">
+        <f aca="false">(F36-80000000)/80000000</f>
+        <v>-0.995796416495392</v>
+      </c>
+      <c r="I36" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="J36" s="12" t="n">
+        <v>4880523</v>
+      </c>
+      <c r="K36" s="2" t="n">
+        <v>452</v>
+      </c>
+      <c r="L36" s="12" t="n">
+        <f aca="false">J36/K36*1000</f>
+        <v>10797617.2566372</v>
+      </c>
+      <c r="M36" s="14" t="n">
+        <f aca="false">(K32-K36)/K32</f>
+        <v>-0.102439024390244</v>
+      </c>
+      <c r="N36" s="14" t="n">
+        <f aca="false">(L36-80000000)/80000000</f>
+        <v>-0.865029784292035</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I37" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="J37" s="12" t="n">
+        <v>119060324</v>
+      </c>
+      <c r="K37" s="2" t="n">
+        <v>11322</v>
+      </c>
+      <c r="L37" s="12" t="n">
+        <f aca="false">J37/K37*1000</f>
+        <v>10515838.5444268</v>
+      </c>
+      <c r="M37" s="23" t="n">
+        <f aca="false">(K33-K37)/K33</f>
+        <v>0.0164190774042221</v>
+      </c>
+      <c r="N37" s="14" t="n">
+        <f aca="false">(L37-80000000)/80000000</f>
+        <v>-0.868552018194665</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1743,24 +1872,24 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="5.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="8.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="16.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="5.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="18.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="36" t="n">
+      <c r="A1" s="38" t="n">
         <v>45393</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="C1" s="7" t="s">
         <v>20</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added pre-calculation of rays attacks remove opposite optimization
</commit_message>
<xml_diff>
--- a/docs/Performance.xlsx
+++ b/docs/Performance.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t xml:space="preserve">classic</t>
   </si>
@@ -81,6 +81,12 @@
   </si>
   <si>
     <t xml:space="preserve">opposite optimization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pre-calculation xray attacks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">removed opposite optimization</t>
   </si>
   <si>
     <t xml:space="preserve">stockfish livello 1</t>
@@ -297,7 +303,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -443,6 +449,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="169" fontId="7" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -702,10 +712,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P41"/>
+  <dimension ref="A1:P45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E41" activeCellId="0" sqref="E41"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E45" activeCellId="0" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1959,6 +1969,127 @@
       <c r="N41" s="14" t="n">
         <f aca="false">(L41-80000000)/80000000</f>
         <v>-0.851100145072536</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="16" t="n">
+        <v>45578</v>
+      </c>
+      <c r="B43" s="17"/>
+      <c r="C43" s="18" t="n">
+        <v>4</v>
+      </c>
+      <c r="D43" s="19" t="n">
+        <v>206603</v>
+      </c>
+      <c r="E43" s="20" t="n">
+        <v>515</v>
+      </c>
+      <c r="F43" s="19" t="n">
+        <f aca="false">D43/E43*1000</f>
+        <v>401170.873786408</v>
+      </c>
+      <c r="G43" s="35" t="n">
+        <f aca="false">(E39-E43)/E39</f>
+        <v>0.0770609318996416</v>
+      </c>
+      <c r="H43" s="22" t="n">
+        <f aca="false">(F43-80000000)/80000000</f>
+        <v>-0.99498536407767</v>
+      </c>
+      <c r="I43" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="J43" s="19" t="n">
+        <v>197281</v>
+      </c>
+      <c r="K43" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="L43" s="19" t="n">
+        <f aca="false">J43/K43*1000</f>
+        <v>13152066.6666667</v>
+      </c>
+      <c r="M43" s="35" t="n">
+        <f aca="false">(K39-K43)/K39</f>
+        <v>0.0625</v>
+      </c>
+      <c r="N43" s="22" t="n">
+        <f aca="false">(L43-80000000)/80000000</f>
+        <v>-0.835599166666667</v>
+      </c>
+      <c r="P43" s="37" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C44" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="D44" s="2" t="n">
+        <v>5072212</v>
+      </c>
+      <c r="E44" s="2" t="n">
+        <v>12788</v>
+      </c>
+      <c r="F44" s="12" t="n">
+        <f aca="false">D44/E44*1000</f>
+        <v>396638.411010322</v>
+      </c>
+      <c r="G44" s="23" t="n">
+        <f aca="false">(E40-E44)/E40</f>
+        <v>0.0735347388248931</v>
+      </c>
+      <c r="H44" s="14" t="n">
+        <f aca="false">(F44-80000000)/80000000</f>
+        <v>-0.995042019862371</v>
+      </c>
+      <c r="I44" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="J44" s="12" t="n">
+        <v>4880523</v>
+      </c>
+      <c r="K44" s="2" t="n">
+        <v>379</v>
+      </c>
+      <c r="L44" s="12" t="n">
+        <f aca="false">J44/K44*1000</f>
+        <v>12877369.3931398</v>
+      </c>
+      <c r="M44" s="23" t="n">
+        <f aca="false">(K40-K44)/K40</f>
+        <v>0.0548628428927681</v>
+      </c>
+      <c r="N44" s="14" t="n">
+        <f aca="false">(L44-80000000)/80000000</f>
+        <v>-0.839032882585752</v>
+      </c>
+      <c r="P44" s="37" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I45" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="J45" s="12" t="n">
+        <v>119060324</v>
+      </c>
+      <c r="K45" s="2" t="n">
+        <v>9359</v>
+      </c>
+      <c r="L45" s="12" t="n">
+        <f aca="false">J45/K45*1000</f>
+        <v>12721479.2178652</v>
+      </c>
+      <c r="M45" s="23" t="n">
+        <f aca="false">(K41-K45)/K41</f>
+        <v>0.063631815907954</v>
+      </c>
+      <c r="N45" s="14" t="n">
+        <f aca="false">(L45-80000000)/80000000</f>
+        <v>-0.840981509776686</v>
       </c>
     </row>
   </sheetData>
@@ -1996,17 +2127,17 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="37" t="n">
+      <c r="A1" s="38" t="n">
         <v>45393</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added pre-calculated attack positions for knight and king moved and optimized castling management
</commit_message>
<xml_diff>
--- a/docs/Performance.xlsx
+++ b/docs/Performance.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t xml:space="preserve">classic</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t xml:space="preserve">removed opposite optimization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moved castling to board</t>
   </si>
   <si>
     <t xml:space="preserve">stockfish livello 1</t>
@@ -712,10 +715,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P45"/>
+  <dimension ref="A1:P49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E45" activeCellId="0" sqref="E45"/>
+      <selection pane="topLeft" activeCell="E49" activeCellId="0" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2018,7 +2021,7 @@
         <f aca="false">(L43-80000000)/80000000</f>
         <v>-0.835599166666667</v>
       </c>
-      <c r="P43" s="37" t="s">
+      <c r="P43" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2065,7 +2068,7 @@
         <f aca="false">(L44-80000000)/80000000</f>
         <v>-0.839032882585752</v>
       </c>
-      <c r="P44" s="37" t="s">
+      <c r="P44" s="7" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2090,6 +2093,124 @@
       <c r="N45" s="14" t="n">
         <f aca="false">(L45-80000000)/80000000</f>
         <v>-0.840981509776686</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="16" t="n">
+        <v>45584</v>
+      </c>
+      <c r="B47" s="17"/>
+      <c r="C47" s="18" t="n">
+        <v>4</v>
+      </c>
+      <c r="D47" s="19" t="n">
+        <v>206603</v>
+      </c>
+      <c r="E47" s="20" t="n">
+        <v>493</v>
+      </c>
+      <c r="F47" s="19" t="n">
+        <f aca="false">D47/E47*1000</f>
+        <v>419073.022312373</v>
+      </c>
+      <c r="G47" s="35" t="n">
+        <f aca="false">(E43-E47)/E43</f>
+        <v>0.0427184466019418</v>
+      </c>
+      <c r="H47" s="22" t="n">
+        <f aca="false">(F47-80000000)/80000000</f>
+        <v>-0.994761587221095</v>
+      </c>
+      <c r="I47" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="J47" s="19" t="n">
+        <v>197281</v>
+      </c>
+      <c r="K47" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="L47" s="19" t="n">
+        <f aca="false">J47/K47*1000</f>
+        <v>14091500</v>
+      </c>
+      <c r="M47" s="35" t="n">
+        <f aca="false">(K43-K47)/K43</f>
+        <v>0.0666666666666667</v>
+      </c>
+      <c r="N47" s="22" t="n">
+        <f aca="false">(L47-80000000)/80000000</f>
+        <v>-0.82385625</v>
+      </c>
+      <c r="P47" s="37" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C48" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="D48" s="2" t="n">
+        <v>5072212</v>
+      </c>
+      <c r="E48" s="2" t="n">
+        <v>12183</v>
+      </c>
+      <c r="F48" s="12" t="n">
+        <f aca="false">D48/E48*1000</f>
+        <v>416335.221209883</v>
+      </c>
+      <c r="G48" s="23" t="n">
+        <f aca="false">(E44-E48)/E44</f>
+        <v>0.047309978104473</v>
+      </c>
+      <c r="H48" s="14" t="n">
+        <f aca="false">(F48-80000000)/80000000</f>
+        <v>-0.994795809734877</v>
+      </c>
+      <c r="I48" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="J48" s="12" t="n">
+        <v>4880523</v>
+      </c>
+      <c r="K48" s="2" t="n">
+        <v>363</v>
+      </c>
+      <c r="L48" s="12" t="n">
+        <f aca="false">J48/K48*1000</f>
+        <v>13444966.9421488</v>
+      </c>
+      <c r="M48" s="23" t="n">
+        <f aca="false">(K44-K48)/K44</f>
+        <v>0.0422163588390501</v>
+      </c>
+      <c r="N48" s="14" t="n">
+        <f aca="false">(L48-80000000)/80000000</f>
+        <v>-0.831937913223141</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I49" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="J49" s="12" t="n">
+        <v>119060324</v>
+      </c>
+      <c r="K49" s="2" t="n">
+        <v>8957</v>
+      </c>
+      <c r="L49" s="12" t="n">
+        <f aca="false">J49/K49*1000</f>
+        <v>13292433.1807525</v>
+      </c>
+      <c r="M49" s="23" t="n">
+        <f aca="false">(K45-K49)/K45</f>
+        <v>0.0429533069772412</v>
+      </c>
+      <c r="N49" s="14" t="n">
+        <f aca="false">(L49-80000000)/80000000</f>
+        <v>-0.833844585240594</v>
       </c>
     </row>
   </sheetData>
@@ -2131,13 +2252,13 @@
         <v>45393</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
optimized pawn attacks reuse of already calculated opposite and side board fixed pieces counters on players complete release of memory allocation
</commit_message>
<xml_diff>
--- a/docs/Performance.xlsx
+++ b/docs/Performance.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
   <si>
     <t xml:space="preserve">classic</t>
   </si>
@@ -90,6 +90,15 @@
   </si>
   <si>
     <t xml:space="preserve">moved castling to board</t>
+  </si>
+  <si>
+    <t xml:space="preserve">optimized rollback management</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pawn attacks optimization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">board and opposite caching</t>
   </si>
   <si>
     <t xml:space="preserve">stockfish livello 1</t>
@@ -306,7 +315,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -452,10 +461,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="169" fontId="7" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -715,10 +720,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P49"/>
+  <dimension ref="A1:P61"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E49" activeCellId="0" sqref="E49"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E58" activeCellId="0" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2142,7 +2147,7 @@
         <f aca="false">(L47-80000000)/80000000</f>
         <v>-0.82385625</v>
       </c>
-      <c r="P47" s="37" t="s">
+      <c r="P47" s="7" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2211,6 +2216,360 @@
       <c r="N49" s="14" t="n">
         <f aca="false">(L49-80000000)/80000000</f>
         <v>-0.833844585240594</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="16" t="n">
+        <v>45590</v>
+      </c>
+      <c r="B51" s="17"/>
+      <c r="C51" s="18" t="n">
+        <v>4</v>
+      </c>
+      <c r="D51" s="19" t="n">
+        <v>206603</v>
+      </c>
+      <c r="E51" s="20" t="n">
+        <v>470</v>
+      </c>
+      <c r="F51" s="19" t="n">
+        <f aca="false">D51/E51*1000</f>
+        <v>439580.85106383</v>
+      </c>
+      <c r="G51" s="35" t="n">
+        <f aca="false">(E47-E51)/E47</f>
+        <v>0.0466531440162272</v>
+      </c>
+      <c r="H51" s="22" t="n">
+        <f aca="false">(F51-80000000)/80000000</f>
+        <v>-0.994505239361702</v>
+      </c>
+      <c r="I51" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="J51" s="19" t="n">
+        <v>197281</v>
+      </c>
+      <c r="K51" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="L51" s="19" t="n">
+        <f aca="false">J51/K51*1000</f>
+        <v>14091500</v>
+      </c>
+      <c r="M51" s="35" t="n">
+        <f aca="false">(K47-K51)/K47</f>
+        <v>0</v>
+      </c>
+      <c r="N51" s="22" t="n">
+        <f aca="false">(L51-80000000)/80000000</f>
+        <v>-0.82385625</v>
+      </c>
+      <c r="P51" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C52" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="D52" s="2" t="n">
+        <v>5072212</v>
+      </c>
+      <c r="E52" s="2" t="n">
+        <v>11779</v>
+      </c>
+      <c r="F52" s="12" t="n">
+        <f aca="false">D52/E52*1000</f>
+        <v>430614.822990067</v>
+      </c>
+      <c r="G52" s="23" t="n">
+        <f aca="false">(E48-E52)/E48</f>
+        <v>0.0331609619962242</v>
+      </c>
+      <c r="H52" s="14" t="n">
+        <f aca="false">(F52-80000000)/80000000</f>
+        <v>-0.994617314712624</v>
+      </c>
+      <c r="I52" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="J52" s="12" t="n">
+        <v>4880523</v>
+      </c>
+      <c r="K52" s="2" t="n">
+        <v>339</v>
+      </c>
+      <c r="L52" s="12" t="n">
+        <f aca="false">J52/K52*1000</f>
+        <v>14396823.0088496</v>
+      </c>
+      <c r="M52" s="23" t="n">
+        <f aca="false">(K48-K52)/K48</f>
+        <v>0.0661157024793388</v>
+      </c>
+      <c r="N52" s="14" t="n">
+        <f aca="false">(L52-80000000)/80000000</f>
+        <v>-0.82003971238938</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I53" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="J53" s="12" t="n">
+        <v>119060324</v>
+      </c>
+      <c r="K53" s="2" t="n">
+        <v>8589</v>
+      </c>
+      <c r="L53" s="12" t="n">
+        <f aca="false">J53/K53*1000</f>
+        <v>13861954.1273722</v>
+      </c>
+      <c r="M53" s="23" t="n">
+        <f aca="false">(K49-K53)/K49</f>
+        <v>0.041085184771687</v>
+      </c>
+      <c r="N53" s="14" t="n">
+        <f aca="false">(L53-80000000)/80000000</f>
+        <v>-0.826725573407847</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="16" t="n">
+        <v>45590</v>
+      </c>
+      <c r="B55" s="17"/>
+      <c r="C55" s="18" t="n">
+        <v>4</v>
+      </c>
+      <c r="D55" s="19" t="n">
+        <v>206603</v>
+      </c>
+      <c r="E55" s="20" t="n">
+        <v>429</v>
+      </c>
+      <c r="F55" s="19" t="n">
+        <f aca="false">D55/E55*1000</f>
+        <v>481592.074592075</v>
+      </c>
+      <c r="G55" s="35" t="n">
+        <f aca="false">(E51-E55)/E51</f>
+        <v>0.0872340425531915</v>
+      </c>
+      <c r="H55" s="22" t="n">
+        <f aca="false">(F55-80000000)/80000000</f>
+        <v>-0.993980099067599</v>
+      </c>
+      <c r="I55" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="J55" s="19" t="n">
+        <v>197281</v>
+      </c>
+      <c r="K55" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="L55" s="19" t="n">
+        <f aca="false">J55/K55*1000</f>
+        <v>16440083.3333333</v>
+      </c>
+      <c r="M55" s="35" t="n">
+        <f aca="false">(K51-K55)/K51</f>
+        <v>0.142857142857143</v>
+      </c>
+      <c r="N55" s="22" t="n">
+        <f aca="false">(L55-80000000)/80000000</f>
+        <v>-0.794498958333333</v>
+      </c>
+      <c r="P55" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C56" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="D56" s="2" t="n">
+        <v>5072212</v>
+      </c>
+      <c r="E56" s="2" t="n">
+        <v>10588</v>
+      </c>
+      <c r="F56" s="12" t="n">
+        <f aca="false">D56/E56*1000</f>
+        <v>479052.890064224</v>
+      </c>
+      <c r="G56" s="23" t="n">
+        <f aca="false">(E52-E56)/E52</f>
+        <v>0.101112148739282</v>
+      </c>
+      <c r="H56" s="14" t="n">
+        <f aca="false">(F56-80000000)/80000000</f>
+        <v>-0.994011838874197</v>
+      </c>
+      <c r="I56" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="J56" s="12" t="n">
+        <v>4880523</v>
+      </c>
+      <c r="K56" s="2" t="n">
+        <v>294</v>
+      </c>
+      <c r="L56" s="12" t="n">
+        <f aca="false">J56/K56*1000</f>
+        <v>16600418.3673469</v>
+      </c>
+      <c r="M56" s="23" t="n">
+        <f aca="false">(K52-K56)/K52</f>
+        <v>0.132743362831858</v>
+      </c>
+      <c r="N56" s="14" t="n">
+        <f aca="false">(L56-80000000)/80000000</f>
+        <v>-0.792494770408163</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I57" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="J57" s="12" t="n">
+        <v>119060324</v>
+      </c>
+      <c r="K57" s="2" t="n">
+        <v>7334</v>
+      </c>
+      <c r="L57" s="12" t="n">
+        <f aca="false">J57/K57*1000</f>
+        <v>16234022.9070085</v>
+      </c>
+      <c r="M57" s="23" t="n">
+        <f aca="false">(K53-K57)/K53</f>
+        <v>0.146117126557224</v>
+      </c>
+      <c r="N57" s="14" t="n">
+        <f aca="false">(L57-80000000)/80000000</f>
+        <v>-0.797074713662394</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="16" t="n">
+        <v>45590</v>
+      </c>
+      <c r="B59" s="17"/>
+      <c r="C59" s="18" t="n">
+        <v>4</v>
+      </c>
+      <c r="D59" s="19" t="n">
+        <v>206603</v>
+      </c>
+      <c r="E59" s="20" t="n">
+        <v>422</v>
+      </c>
+      <c r="F59" s="19" t="n">
+        <f aca="false">D59/E59*1000</f>
+        <v>489580.568720379</v>
+      </c>
+      <c r="G59" s="35" t="n">
+        <f aca="false">(E55-E59)/E55</f>
+        <v>0.0163170163170163</v>
+      </c>
+      <c r="H59" s="22" t="n">
+        <f aca="false">(F59-80000000)/80000000</f>
+        <v>-0.993880242890995</v>
+      </c>
+      <c r="I59" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="J59" s="19" t="n">
+        <v>197281</v>
+      </c>
+      <c r="K59" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="L59" s="19" t="n">
+        <f aca="false">J59/K59*1000</f>
+        <v>17934636.3636364</v>
+      </c>
+      <c r="M59" s="35" t="n">
+        <f aca="false">(K55-K59)/K55</f>
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="N59" s="22" t="n">
+        <f aca="false">(L59-80000000)/80000000</f>
+        <v>-0.775817045454546</v>
+      </c>
+      <c r="P59" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C60" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="D60" s="2" t="n">
+        <v>5072212</v>
+      </c>
+      <c r="E60" s="2" t="n">
+        <v>10273</v>
+      </c>
+      <c r="F60" s="12" t="n">
+        <f aca="false">D60/E60*1000</f>
+        <v>493742.042246666</v>
+      </c>
+      <c r="G60" s="23" t="n">
+        <f aca="false">(E56-E60)/E56</f>
+        <v>0.0297506611258028</v>
+      </c>
+      <c r="H60" s="14" t="n">
+        <f aca="false">(F60-80000000)/80000000</f>
+        <v>-0.993828224471917</v>
+      </c>
+      <c r="I60" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="J60" s="12" t="n">
+        <v>4880523</v>
+      </c>
+      <c r="K60" s="2" t="n">
+        <v>292</v>
+      </c>
+      <c r="L60" s="12" t="n">
+        <f aca="false">J60/K60*1000</f>
+        <v>16714119.8630137</v>
+      </c>
+      <c r="M60" s="23" t="n">
+        <f aca="false">(K56-K60)/K56</f>
+        <v>0.00680272108843537</v>
+      </c>
+      <c r="N60" s="14" t="n">
+        <f aca="false">(L60-80000000)/80000000</f>
+        <v>-0.791073501712329</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I61" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="J61" s="12" t="n">
+        <v>119060324</v>
+      </c>
+      <c r="K61" s="2" t="n">
+        <v>7042</v>
+      </c>
+      <c r="L61" s="12" t="n">
+        <f aca="false">J61/K61*1000</f>
+        <v>16907174.666288</v>
+      </c>
+      <c r="M61" s="23" t="n">
+        <f aca="false">(K57-K61)/K57</f>
+        <v>0.039814562312517</v>
+      </c>
+      <c r="N61" s="14" t="n">
+        <f aca="false">(L61-80000000)/80000000</f>
+        <v>-0.7886603166714</v>
       </c>
     </row>
   </sheetData>
@@ -2248,17 +2607,17 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="38" t="n">
+      <c r="A1" s="37" t="n">
         <v>45393</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rollbacked ray attacks from branchless version
</commit_message>
<xml_diff>
--- a/docs/Performance.xlsx
+++ b/docs/Performance.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t xml:space="preserve">classic</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t xml:space="preserve">board and opposite caching</t>
+  </si>
+  <si>
+    <t xml:space="preserve">removed branchless on rayattacks</t>
   </si>
   <si>
     <t xml:space="preserve">stockfish livello 1</t>
@@ -315,7 +318,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -461,6 +464,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="169" fontId="7" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -720,10 +727,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P61"/>
+  <dimension ref="A1:R65"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E58" activeCellId="0" sqref="E58"/>
+      <selection pane="topLeft" activeCell="E65" activeCellId="0" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2548,6 +2555,9 @@
         <f aca="false">(L60-80000000)/80000000</f>
         <v>-0.791073501712329</v>
       </c>
+      <c r="R60" s="0" t="n">
+        <v>8900</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I61" s="2" t="n">
@@ -2570,6 +2580,127 @@
       <c r="N61" s="14" t="n">
         <f aca="false">(L61-80000000)/80000000</f>
         <v>-0.7886603166714</v>
+      </c>
+      <c r="R61" s="0" t="n">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="16" t="n">
+        <v>45606</v>
+      </c>
+      <c r="B63" s="17"/>
+      <c r="C63" s="18" t="n">
+        <v>4</v>
+      </c>
+      <c r="D63" s="19" t="n">
+        <v>206603</v>
+      </c>
+      <c r="E63" s="20" t="n">
+        <v>357</v>
+      </c>
+      <c r="F63" s="19" t="n">
+        <f aca="false">D63/E63*1000</f>
+        <v>578719.887955182</v>
+      </c>
+      <c r="G63" s="35" t="n">
+        <f aca="false">(E59-E63)/E59</f>
+        <v>0.154028436018957</v>
+      </c>
+      <c r="H63" s="22" t="n">
+        <f aca="false">(F63-80000000)/80000000</f>
+        <v>-0.99276600140056</v>
+      </c>
+      <c r="I63" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="J63" s="19" t="n">
+        <v>197281</v>
+      </c>
+      <c r="K63" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="L63" s="19" t="n">
+        <f aca="false">J63/K63*1000</f>
+        <v>21920111.1111111</v>
+      </c>
+      <c r="M63" s="35" t="n">
+        <f aca="false">(K59-K63)/K59</f>
+        <v>0.181818181818182</v>
+      </c>
+      <c r="N63" s="22" t="n">
+        <f aca="false">(L63-80000000)/80000000</f>
+        <v>-0.725998611111111</v>
+      </c>
+      <c r="P63" s="37" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C64" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="D64" s="2" t="n">
+        <v>5072212</v>
+      </c>
+      <c r="E64" s="2" t="n">
+        <v>9165</v>
+      </c>
+      <c r="F64" s="12" t="n">
+        <f aca="false">D64/E64*1000</f>
+        <v>553432.84233497</v>
+      </c>
+      <c r="G64" s="23" t="n">
+        <f aca="false">(E60-E64)/E60</f>
+        <v>0.107855543658133</v>
+      </c>
+      <c r="H64" s="14" t="n">
+        <f aca="false">(F64-80000000)/80000000</f>
+        <v>-0.993082089470813</v>
+      </c>
+      <c r="I64" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="J64" s="12" t="n">
+        <v>4880523</v>
+      </c>
+      <c r="K64" s="2" t="n">
+        <v>221</v>
+      </c>
+      <c r="L64" s="12" t="n">
+        <f aca="false">J64/K64*1000</f>
+        <v>22083814.479638</v>
+      </c>
+      <c r="M64" s="23" t="n">
+        <f aca="false">(K60-K64)/K60</f>
+        <v>0.243150684931507</v>
+      </c>
+      <c r="N64" s="14" t="n">
+        <f aca="false">(L64-80000000)/80000000</f>
+        <v>-0.723952319004525</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I65" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="J65" s="12" t="n">
+        <v>119060324</v>
+      </c>
+      <c r="K65" s="2" t="n">
+        <v>5889</v>
+      </c>
+      <c r="L65" s="12" t="n">
+        <f aca="false">J65/K65*1000</f>
+        <v>20217409.4073697</v>
+      </c>
+      <c r="M65" s="23" t="n">
+        <f aca="false">(K61-K65)/K61</f>
+        <v>0.163731894348197</v>
+      </c>
+      <c r="N65" s="14" t="n">
+        <f aca="false">(L65-80000000)/80000000</f>
+        <v>-0.747282382407879</v>
       </c>
     </row>
   </sheetData>
@@ -2607,17 +2738,17 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="37" t="n">
+      <c r="A1" s="38" t="n">
         <v>45393</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added array pool added use of array also in moves generator fixed tests with exceptions refactored performance test class wip new moves cache wip vector vs array pool
</commit_message>
<xml_diff>
--- a/docs/Performance.xlsx
+++ b/docs/Performance.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t xml:space="preserve">classic</t>
   </si>
@@ -102,6 +102,12 @@
   </si>
   <si>
     <t xml:space="preserve">removed branchless on rayattacks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">replaced pool vector with pool array (no board and opposite caching)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(5932 with board and opposite caching)</t>
   </si>
   <si>
     <t xml:space="preserve">stockfish livello 1</t>
@@ -318,7 +324,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -464,10 +470,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="169" fontId="7" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -727,13 +729,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R65"/>
+  <dimension ref="A1:R69"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E65" activeCellId="0" sqref="E65"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A23" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P69" activeCellId="0" sqref="P69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="16.1484375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="11.57"/>
@@ -2555,9 +2557,7 @@
         <f aca="false">(L60-80000000)/80000000</f>
         <v>-0.791073501712329</v>
       </c>
-      <c r="R60" s="0" t="n">
-        <v>8900</v>
-      </c>
+      <c r="R60" s="2"/>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I61" s="2" t="n">
@@ -2581,9 +2581,7 @@
         <f aca="false">(L61-80000000)/80000000</f>
         <v>-0.7886603166714</v>
       </c>
-      <c r="R61" s="0" t="n">
-        <v>210</v>
-      </c>
+      <c r="R61" s="2"/>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="16" t="n">
@@ -2632,7 +2630,7 @@
         <f aca="false">(L63-80000000)/80000000</f>
         <v>-0.725998611111111</v>
       </c>
-      <c r="P63" s="37" t="s">
+      <c r="P63" s="7" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2701,6 +2699,127 @@
       <c r="N65" s="14" t="n">
         <f aca="false">(L65-80000000)/80000000</f>
         <v>-0.747282382407879</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="16" t="n">
+        <v>45862</v>
+      </c>
+      <c r="B67" s="17"/>
+      <c r="C67" s="18" t="n">
+        <v>4</v>
+      </c>
+      <c r="D67" s="19" t="n">
+        <v>206603</v>
+      </c>
+      <c r="E67" s="20" t="n">
+        <v>274</v>
+      </c>
+      <c r="F67" s="19" t="n">
+        <f aca="false">D67/E67*1000</f>
+        <v>754025.547445255</v>
+      </c>
+      <c r="G67" s="35" t="n">
+        <f aca="false">(E63-E67)/E63</f>
+        <v>0.23249299719888</v>
+      </c>
+      <c r="H67" s="22" t="n">
+        <f aca="false">(F67-80000000)/80000000</f>
+        <v>-0.990574680656934</v>
+      </c>
+      <c r="I67" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="J67" s="19" t="n">
+        <v>197281</v>
+      </c>
+      <c r="K67" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="L67" s="19" t="n">
+        <f aca="false">J67/K67*1000</f>
+        <v>21920111.1111111</v>
+      </c>
+      <c r="M67" s="35" t="n">
+        <f aca="false">(K63-K67)/K63</f>
+        <v>0</v>
+      </c>
+      <c r="N67" s="22" t="n">
+        <f aca="false">(L67-80000000)/80000000</f>
+        <v>-0.725998611111111</v>
+      </c>
+      <c r="P67" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C68" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="D68" s="2" t="n">
+        <v>5072212</v>
+      </c>
+      <c r="E68" s="2" t="n">
+        <v>7220</v>
+      </c>
+      <c r="F68" s="12" t="n">
+        <f aca="false">D68/E68*1000</f>
+        <v>702522.43767313</v>
+      </c>
+      <c r="G68" s="23" t="n">
+        <f aca="false">(E64-E68)/E64</f>
+        <v>0.212220403709765</v>
+      </c>
+      <c r="H68" s="14" t="n">
+        <f aca="false">(F68-80000000)/80000000</f>
+        <v>-0.991218469529086</v>
+      </c>
+      <c r="I68" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="J68" s="12" t="n">
+        <v>4880523</v>
+      </c>
+      <c r="K68" s="2" t="n">
+        <v>223</v>
+      </c>
+      <c r="L68" s="12" t="n">
+        <f aca="false">J68/K68*1000</f>
+        <v>21885753.3632287</v>
+      </c>
+      <c r="M68" s="14" t="n">
+        <f aca="false">(K64-K68)/K64</f>
+        <v>-0.00904977375565611</v>
+      </c>
+      <c r="N68" s="14" t="n">
+        <f aca="false">(L68-80000000)/80000000</f>
+        <v>-0.726428082959641</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I69" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="J69" s="12" t="n">
+        <v>119060324</v>
+      </c>
+      <c r="K69" s="2" t="n">
+        <v>5953</v>
+      </c>
+      <c r="L69" s="12" t="n">
+        <f aca="false">J69/K69*1000</f>
+        <v>20000054.4263397</v>
+      </c>
+      <c r="M69" s="14" t="n">
+        <f aca="false">(K65-K69)/K65</f>
+        <v>-0.010867719476991</v>
+      </c>
+      <c r="N69" s="14" t="n">
+        <f aca="false">(L69-80000000)/80000000</f>
+        <v>-0.749999319670754</v>
+      </c>
+      <c r="P69" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -2729,7 +2848,7 @@
       <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.1484375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="8.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="16.43"/>
@@ -2738,17 +2857,17 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="38" t="n">
+      <c r="A1" s="37" t="n">
         <v>45393</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
completed transition from vector to array added abstract engine class that includes common features
</commit_message>
<xml_diff>
--- a/docs/Performance.xlsx
+++ b/docs/Performance.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
   <si>
     <t xml:space="preserve">classic</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t xml:space="preserve">(5932 with board and opposite caching)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moves cache array</t>
   </si>
   <si>
     <t xml:space="preserve">stockfish livello 1</t>
@@ -729,10 +732,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R69"/>
+  <dimension ref="A1:R74"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A23" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P69" activeCellId="0" sqref="P69"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K75" activeCellId="0" sqref="K75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.1484375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2748,7 +2751,7 @@
         <f aca="false">(L67-80000000)/80000000</f>
         <v>-0.725998611111111</v>
       </c>
-      <c r="P67" s="0" t="s">
+      <c r="P67" s="2" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2760,19 +2763,19 @@
         <v>5072212</v>
       </c>
       <c r="E68" s="2" t="n">
-        <v>7220</v>
+        <v>7448</v>
       </c>
       <c r="F68" s="12" t="n">
         <f aca="false">D68/E68*1000</f>
-        <v>702522.43767313</v>
+        <v>681016.648764769</v>
       </c>
       <c r="G68" s="23" t="n">
         <f aca="false">(E64-E68)/E64</f>
-        <v>0.212220403709765</v>
+        <v>0.1873431533006</v>
       </c>
       <c r="H68" s="14" t="n">
         <f aca="false">(F68-80000000)/80000000</f>
-        <v>-0.991218469529086</v>
+        <v>-0.99148729189044</v>
       </c>
       <c r="I68" s="2" t="n">
         <v>5</v>
@@ -2818,8 +2821,164 @@
         <f aca="false">(L69-80000000)/80000000</f>
         <v>-0.749999319670754</v>
       </c>
-      <c r="P69" s="0" t="s">
+      <c r="P69" s="2" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A71" s="26" t="n">
+        <v>45873</v>
+      </c>
+      <c r="B71" s="27"/>
+      <c r="C71" s="28" t="n">
+        <v>4</v>
+      </c>
+      <c r="D71" s="29" t="n">
+        <v>206603</v>
+      </c>
+      <c r="E71" s="30" t="n">
+        <v>280</v>
+      </c>
+      <c r="F71" s="29" t="n">
+        <f aca="false">D71/E71*1000</f>
+        <v>737867.857142857</v>
+      </c>
+      <c r="G71" s="24" t="n">
+        <f aca="false">(E67-E71)/E67</f>
+        <v>-0.0218978102189781</v>
+      </c>
+      <c r="H71" s="22" t="n">
+        <f aca="false">(F71-80000000)/80000000</f>
+        <v>-0.990776651785714</v>
+      </c>
+      <c r="I71" s="31" t="n">
+        <v>4</v>
+      </c>
+      <c r="J71" s="29" t="n">
+        <v>197281</v>
+      </c>
+      <c r="K71" s="31" t="n">
+        <v>13</v>
+      </c>
+      <c r="L71" s="29" t="n">
+        <f aca="false">J71/K71*1000</f>
+        <v>15175461.5384615</v>
+      </c>
+      <c r="M71" s="22" t="n">
+        <f aca="false">(K67-K71)/K67</f>
+        <v>-0.444444444444444</v>
+      </c>
+      <c r="N71" s="22" t="n">
+        <f aca="false">(L71-80000000)/80000000</f>
+        <v>-0.810306730769231</v>
+      </c>
+      <c r="P71" s="32" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A72" s="32"/>
+      <c r="B72" s="33"/>
+      <c r="C72" s="32" t="n">
+        <v>5</v>
+      </c>
+      <c r="D72" s="32" t="n">
+        <v>5072212</v>
+      </c>
+      <c r="E72" s="32" t="n">
+        <v>6070</v>
+      </c>
+      <c r="F72" s="34" t="n">
+        <f aca="false">D72/E72*1000</f>
+        <v>835619.769357496</v>
+      </c>
+      <c r="G72" s="23" t="n">
+        <f aca="false">(E68-E72)/E68</f>
+        <v>0.185016111707841</v>
+      </c>
+      <c r="H72" s="14" t="n">
+        <f aca="false">(F72-80000000)/80000000</f>
+        <v>-0.989554752883031</v>
+      </c>
+      <c r="I72" s="32" t="n">
+        <v>5</v>
+      </c>
+      <c r="J72" s="34" t="n">
+        <v>4880523</v>
+      </c>
+      <c r="K72" s="32" t="n">
+        <v>229</v>
+      </c>
+      <c r="L72" s="34" t="n">
+        <f aca="false">J72/K72*1000</f>
+        <v>21312327.510917</v>
+      </c>
+      <c r="M72" s="14" t="n">
+        <f aca="false">(K68-K72)/K68</f>
+        <v>-0.0269058295964126</v>
+      </c>
+      <c r="N72" s="14" t="n">
+        <f aca="false">(L72-80000000)/80000000</f>
+        <v>-0.733595906113537</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A73" s="32"/>
+      <c r="B73" s="33"/>
+      <c r="C73" s="32"/>
+      <c r="D73" s="32"/>
+      <c r="E73" s="32"/>
+      <c r="F73" s="32"/>
+      <c r="G73" s="32"/>
+      <c r="H73" s="33"/>
+      <c r="I73" s="32" t="n">
+        <v>6</v>
+      </c>
+      <c r="J73" s="34" t="n">
+        <v>119060324</v>
+      </c>
+      <c r="K73" s="32" t="n">
+        <v>4920</v>
+      </c>
+      <c r="L73" s="34" t="n">
+        <f aca="false">J73/K73*1000</f>
+        <v>24199252.8455285</v>
+      </c>
+      <c r="M73" s="23" t="n">
+        <f aca="false">(K69-K73)/K69</f>
+        <v>0.173525953300857</v>
+      </c>
+      <c r="N73" s="14" t="n">
+        <f aca="false">(L73-80000000)/80000000</f>
+        <v>-0.697509339430894</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A74" s="32"/>
+      <c r="B74" s="33"/>
+      <c r="C74" s="32"/>
+      <c r="D74" s="32"/>
+      <c r="E74" s="32"/>
+      <c r="F74" s="32"/>
+      <c r="G74" s="32"/>
+      <c r="H74" s="33"/>
+      <c r="I74" s="32" t="n">
+        <v>7</v>
+      </c>
+      <c r="J74" s="34" t="n">
+        <v>3195901860</v>
+      </c>
+      <c r="K74" s="32" t="n">
+        <v>110737</v>
+      </c>
+      <c r="L74" s="34" t="n">
+        <f aca="false">J74/K74*1000</f>
+        <v>28860289.3341882</v>
+      </c>
+      <c r="M74" s="32"/>
+      <c r="N74" s="25" t="n">
+        <f aca="false">(L74-80000000)/80000000</f>
+        <v>-0.639246383322647</v>
       </c>
     </row>
   </sheetData>
@@ -2861,13 +3020,13 @@
         <v>45393</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactored MovesAmount to a struct
</commit_message>
<xml_diff>
--- a/docs/Performance.xlsx
+++ b/docs/Performance.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t xml:space="preserve">classic</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t xml:space="preserve">moves cache array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">removed moves calculation from board class</t>
   </si>
   <si>
     <t xml:space="preserve">stockfish livello 1</t>
@@ -327,7 +330,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -473,6 +476,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="169" fontId="7" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="8" fillId="4" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -732,10 +739,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R74"/>
+  <dimension ref="A1:R78"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K75" activeCellId="0" sqref="K75"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F77" activeCellId="0" sqref="F77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.1484375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2979,6 +2986,124 @@
       <c r="N74" s="25" t="n">
         <f aca="false">(L74-80000000)/80000000</f>
         <v>-0.639246383322647</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A76" s="16" t="n">
+        <v>45956</v>
+      </c>
+      <c r="B76" s="17"/>
+      <c r="C76" s="18" t="n">
+        <v>4</v>
+      </c>
+      <c r="D76" s="19" t="n">
+        <v>206603</v>
+      </c>
+      <c r="E76" s="20" t="n">
+        <v>275</v>
+      </c>
+      <c r="F76" s="19" t="n">
+        <f aca="false">D76/E76*1000</f>
+        <v>751283.636363636</v>
+      </c>
+      <c r="G76" s="22" t="n">
+        <f aca="false">(E67-E76)/E67</f>
+        <v>-0.00364963503649635</v>
+      </c>
+      <c r="H76" s="22" t="n">
+        <f aca="false">(F76-80000000)/80000000</f>
+        <v>-0.990608954545455</v>
+      </c>
+      <c r="I76" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="J76" s="19" t="n">
+        <v>197281</v>
+      </c>
+      <c r="K76" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="L76" s="19" t="n">
+        <f aca="false">J76/K76*1000</f>
+        <v>21920111.1111111</v>
+      </c>
+      <c r="M76" s="35" t="n">
+        <f aca="false">(K67-K76)/K67</f>
+        <v>0</v>
+      </c>
+      <c r="N76" s="22" t="n">
+        <f aca="false">(L76-80000000)/80000000</f>
+        <v>-0.725998611111111</v>
+      </c>
+      <c r="P76" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C77" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="D77" s="2" t="n">
+        <v>5072212</v>
+      </c>
+      <c r="E77" s="2" t="n">
+        <v>7015</v>
+      </c>
+      <c r="F77" s="12" t="n">
+        <f aca="false">D77/E77*1000</f>
+        <v>723052.316464719</v>
+      </c>
+      <c r="G77" s="23" t="n">
+        <f aca="false">(E68-E77)/E68</f>
+        <v>0.0581364124597207</v>
+      </c>
+      <c r="H77" s="14" t="n">
+        <f aca="false">(F77-80000000)/80000000</f>
+        <v>-0.990961846044191</v>
+      </c>
+      <c r="I77" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="J77" s="12" t="n">
+        <v>4880523</v>
+      </c>
+      <c r="K77" s="2" t="n">
+        <v>230</v>
+      </c>
+      <c r="L77" s="12" t="n">
+        <f aca="false">J77/K77*1000</f>
+        <v>21219665.2173913</v>
+      </c>
+      <c r="M77" s="14" t="n">
+        <f aca="false">(K68-K77)/K68</f>
+        <v>-0.031390134529148</v>
+      </c>
+      <c r="N77" s="14" t="n">
+        <f aca="false">(L77-80000000)/80000000</f>
+        <v>-0.734754184782609</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I78" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="J78" s="12" t="n">
+        <v>119060324</v>
+      </c>
+      <c r="K78" s="2" t="n">
+        <v>5862</v>
+      </c>
+      <c r="L78" s="12" t="n">
+        <f aca="false">J78/K78*1000</f>
+        <v>20310529.5121119</v>
+      </c>
+      <c r="M78" s="37" t="n">
+        <f aca="false">(K69-K78)/K69</f>
+        <v>0.0152864102133378</v>
+      </c>
+      <c r="N78" s="14" t="n">
+        <f aca="false">(L78-80000000)/80000000</f>
+        <v>-0.746118381098601</v>
       </c>
     </row>
   </sheetData>
@@ -3016,17 +3141,17 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="37" t="n">
+      <c r="A1" s="38" t="n">
         <v>45393</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
replaced unsigned char with unsigned int
</commit_message>
<xml_diff>
--- a/docs/Performance.xlsx
+++ b/docs/Performance.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
   <si>
     <t xml:space="preserve">classic</t>
   </si>
@@ -114,6 +114,15 @@
   </si>
   <si>
     <t xml:space="preserve">removed moves calculation from board class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">added functions map for destination calculation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">added pawn attacks functional maps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">replaced unsigned char with unsigned int</t>
   </si>
   <si>
     <t xml:space="preserve">stockfish livello 1</t>
@@ -739,10 +748,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R78"/>
+  <dimension ref="A1:R82"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F77" activeCellId="0" sqref="F77"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A42" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F82" activeCellId="0" sqref="F82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.1484375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3035,7 +3044,7 @@
         <f aca="false">(L76-80000000)/80000000</f>
         <v>-0.725998611111111</v>
       </c>
-      <c r="P76" s="0" t="s">
+      <c r="P76" s="2" t="s">
         <v>30</v>
       </c>
     </row>
@@ -3082,6 +3091,9 @@
         <f aca="false">(L77-80000000)/80000000</f>
         <v>-0.734754184782609</v>
       </c>
+      <c r="P77" s="0" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="I78" s="2" t="n">
@@ -3104,6 +3116,127 @@
       <c r="N78" s="14" t="n">
         <f aca="false">(L78-80000000)/80000000</f>
         <v>-0.746118381098601</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A80" s="16" t="n">
+        <v>45961</v>
+      </c>
+      <c r="B80" s="17"/>
+      <c r="C80" s="18" t="n">
+        <v>4</v>
+      </c>
+      <c r="D80" s="19" t="n">
+        <v>206603</v>
+      </c>
+      <c r="E80" s="20" t="n">
+        <v>249</v>
+      </c>
+      <c r="F80" s="19" t="n">
+        <f aca="false">D80/E80*1000</f>
+        <v>829730.923694779</v>
+      </c>
+      <c r="G80" s="35" t="n">
+        <f aca="false">(E76-E80)/E76</f>
+        <v>0.0945454545454545</v>
+      </c>
+      <c r="H80" s="22" t="n">
+        <f aca="false">(F80-80000000)/80000000</f>
+        <v>-0.989628363453815</v>
+      </c>
+      <c r="I80" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="J80" s="19" t="n">
+        <v>197281</v>
+      </c>
+      <c r="K80" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="L80" s="19" t="n">
+        <f aca="false">J80/K80*1000</f>
+        <v>21920111.1111111</v>
+      </c>
+      <c r="M80" s="35" t="n">
+        <f aca="false">(K76-K80)/K76</f>
+        <v>0</v>
+      </c>
+      <c r="N80" s="22" t="n">
+        <f aca="false">(L80-80000000)/80000000</f>
+        <v>-0.725998611111111</v>
+      </c>
+      <c r="P80" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C81" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="D81" s="2" t="n">
+        <v>5072212</v>
+      </c>
+      <c r="E81" s="2" t="n">
+        <v>6742</v>
+      </c>
+      <c r="F81" s="12" t="n">
+        <f aca="false">D81/E81*1000</f>
+        <v>752330.46573717</v>
+      </c>
+      <c r="G81" s="23" t="n">
+        <f aca="false">(E77-E81)/E77</f>
+        <v>0.0389166072701354</v>
+      </c>
+      <c r="H81" s="14" t="n">
+        <f aca="false">(F81-80000000)/80000000</f>
+        <v>-0.990595869178286</v>
+      </c>
+      <c r="I81" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="J81" s="12" t="n">
+        <v>4880523</v>
+      </c>
+      <c r="K81" s="2" t="n">
+        <v>206</v>
+      </c>
+      <c r="L81" s="12" t="n">
+        <f aca="false">J81/K81*1000</f>
+        <v>23691859.223301</v>
+      </c>
+      <c r="M81" s="37" t="n">
+        <f aca="false">(K77-K81)/K77</f>
+        <v>0.104347826086957</v>
+      </c>
+      <c r="N81" s="14" t="n">
+        <f aca="false">(L81-80000000)/80000000</f>
+        <v>-0.703851759708738</v>
+      </c>
+      <c r="P81" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I82" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="J82" s="12" t="n">
+        <v>119060324</v>
+      </c>
+      <c r="K82" s="2" t="n">
+        <v>5611</v>
+      </c>
+      <c r="L82" s="12" t="n">
+        <f aca="false">J82/K82*1000</f>
+        <v>21219091.7839957</v>
+      </c>
+      <c r="M82" s="37" t="n">
+        <f aca="false">(K78-K82)/K78</f>
+        <v>0.0428181508017741</v>
+      </c>
+      <c r="N82" s="14" t="n">
+        <f aca="false">(L82-80000000)/80000000</f>
+        <v>-0.734761352700054</v>
       </c>
     </row>
   </sheetData>
@@ -3145,13 +3278,13 @@
         <v>45393</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
on move validation, avoided obvious ray attacks calculation
</commit_message>
<xml_diff>
--- a/docs/Performance.xlsx
+++ b/docs/Performance.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
   <si>
     <t xml:space="preserve">classic</t>
   </si>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t xml:space="preserve">replaced unsigned char with unsigned int</t>
+  </si>
+  <si>
+    <t xml:space="preserve">avoided obvious ray attacks calculation on move validation</t>
   </si>
   <si>
     <t xml:space="preserve">stockfish livello 1</t>
@@ -748,10 +751,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R82"/>
+  <dimension ref="A1:R86"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A42" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F82" activeCellId="0" sqref="F82"/>
+      <selection pane="topLeft" activeCell="P85" activeCellId="0" sqref="P85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.1484375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3091,7 +3094,7 @@
         <f aca="false">(L77-80000000)/80000000</f>
         <v>-0.734754184782609</v>
       </c>
-      <c r="P77" s="0" t="s">
+      <c r="P77" s="2" t="s">
         <v>31</v>
       </c>
     </row>
@@ -3165,7 +3168,7 @@
         <f aca="false">(L80-80000000)/80000000</f>
         <v>-0.725998611111111</v>
       </c>
-      <c r="P80" s="0" t="s">
+      <c r="P80" s="2" t="s">
         <v>32</v>
       </c>
     </row>
@@ -3212,7 +3215,7 @@
         <f aca="false">(L81-80000000)/80000000</f>
         <v>-0.703851759708738</v>
       </c>
-      <c r="P81" s="0" t="s">
+      <c r="P81" s="2" t="s">
         <v>33</v>
       </c>
     </row>
@@ -3237,6 +3240,124 @@
       <c r="N82" s="14" t="n">
         <f aca="false">(L82-80000000)/80000000</f>
         <v>-0.734761352700054</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A84" s="16" t="n">
+        <v>45970</v>
+      </c>
+      <c r="B84" s="17"/>
+      <c r="C84" s="18" t="n">
+        <v>4</v>
+      </c>
+      <c r="D84" s="19" t="n">
+        <v>206603</v>
+      </c>
+      <c r="E84" s="20" t="n">
+        <v>206</v>
+      </c>
+      <c r="F84" s="19" t="n">
+        <f aca="false">D84/E84*1000</f>
+        <v>1002927.18446602</v>
+      </c>
+      <c r="G84" s="35" t="n">
+        <f aca="false">(E80-E84)/E80</f>
+        <v>0.172690763052209</v>
+      </c>
+      <c r="H84" s="22" t="n">
+        <f aca="false">(F84-80000000)/80000000</f>
+        <v>-0.987463410194175</v>
+      </c>
+      <c r="I84" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="J84" s="19" t="n">
+        <v>197281</v>
+      </c>
+      <c r="K84" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="L84" s="19" t="n">
+        <f aca="false">J84/K84*1000</f>
+        <v>32880166.6666667</v>
+      </c>
+      <c r="M84" s="35" t="n">
+        <f aca="false">(K80-K84)/K80</f>
+        <v>0.333333333333333</v>
+      </c>
+      <c r="N84" s="22" t="n">
+        <f aca="false">(L84-80000000)/80000000</f>
+        <v>-0.588997916666667</v>
+      </c>
+      <c r="P84" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C85" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="D85" s="2" t="n">
+        <v>5072212</v>
+      </c>
+      <c r="E85" s="2" t="n">
+        <v>5048</v>
+      </c>
+      <c r="F85" s="12" t="n">
+        <f aca="false">D85/E85*1000</f>
+        <v>1004796.35499208</v>
+      </c>
+      <c r="G85" s="23" t="n">
+        <f aca="false">(E81-E85)/E81</f>
+        <v>0.251260753485613</v>
+      </c>
+      <c r="H85" s="14" t="n">
+        <f aca="false">(F85-80000000)/80000000</f>
+        <v>-0.987440045562599</v>
+      </c>
+      <c r="I85" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="J85" s="12" t="n">
+        <v>4880523</v>
+      </c>
+      <c r="K85" s="2" t="n">
+        <v>155</v>
+      </c>
+      <c r="L85" s="12" t="n">
+        <f aca="false">J85/K85*1000</f>
+        <v>31487245.1612903</v>
+      </c>
+      <c r="M85" s="37" t="n">
+        <f aca="false">(K81-K85)/K81</f>
+        <v>0.247572815533981</v>
+      </c>
+      <c r="N85" s="14" t="n">
+        <f aca="false">(L85-80000000)/80000000</f>
+        <v>-0.606409435483871</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I86" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="J86" s="12" t="n">
+        <v>119060324</v>
+      </c>
+      <c r="K86" s="2" t="n">
+        <v>3790</v>
+      </c>
+      <c r="L86" s="12" t="n">
+        <f aca="false">J86/K86*1000</f>
+        <v>31414333.5092348</v>
+      </c>
+      <c r="M86" s="37" t="n">
+        <f aca="false">(K82-K86)/K82</f>
+        <v>0.324541080021387</v>
+      </c>
+      <c r="N86" s="14" t="n">
+        <f aca="false">(L86-80000000)/80000000</f>
+        <v>-0.607320831134565</v>
       </c>
     </row>
   </sheetData>
@@ -3278,13 +3399,13 @@
         <v>45393</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
on verify checks, avoided obvious ray attacks calculation
</commit_message>
<xml_diff>
--- a/docs/Performance.xlsx
+++ b/docs/Performance.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
   <si>
     <t xml:space="preserve">classic</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t xml:space="preserve">avoided obvious ray attacks calculation on move validation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">avoided obvious ray attacks calculation on verify checks</t>
   </si>
   <si>
     <t xml:space="preserve">stockfish livello 1</t>
@@ -751,10 +754,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R86"/>
+  <dimension ref="A1:R90"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A42" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P85" activeCellId="0" sqref="P85"/>
+      <selection pane="topLeft" activeCell="E89" activeCellId="0" sqref="E89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.1484375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2809,7 +2812,7 @@
         <f aca="false">J68/K68*1000</f>
         <v>21885753.3632287</v>
       </c>
-      <c r="M68" s="14" t="n">
+      <c r="M68" s="25" t="n">
         <f aca="false">(K64-K68)/K64</f>
         <v>-0.00904977375565611</v>
       </c>
@@ -2832,7 +2835,7 @@
         <f aca="false">J69/K69*1000</f>
         <v>20000054.4263397</v>
       </c>
-      <c r="M69" s="14" t="n">
+      <c r="M69" s="25" t="n">
         <f aca="false">(K65-K69)/K65</f>
         <v>-0.010867719476991</v>
       </c>
@@ -2883,7 +2886,7 @@
         <f aca="false">J71/K71*1000</f>
         <v>15175461.5384615</v>
       </c>
-      <c r="M71" s="22" t="n">
+      <c r="M71" s="24" t="n">
         <f aca="false">(K67-K71)/K67</f>
         <v>-0.444444444444444</v>
       </c>
@@ -2932,7 +2935,7 @@
         <f aca="false">J72/K72*1000</f>
         <v>21312327.510917</v>
       </c>
-      <c r="M72" s="14" t="n">
+      <c r="M72" s="25" t="n">
         <f aca="false">(K68-K72)/K68</f>
         <v>-0.0269058295964126</v>
       </c>
@@ -3018,7 +3021,7 @@
         <f aca="false">D76/E76*1000</f>
         <v>751283.636363636</v>
       </c>
-      <c r="G76" s="22" t="n">
+      <c r="G76" s="24" t="n">
         <f aca="false">(E67-E76)/E67</f>
         <v>-0.00364963503649635</v>
       </c>
@@ -3086,7 +3089,7 @@
         <f aca="false">J77/K77*1000</f>
         <v>21219665.2173913</v>
       </c>
-      <c r="M77" s="14" t="n">
+      <c r="M77" s="25" t="n">
         <f aca="false">(K68-K77)/K68</f>
         <v>-0.031390134529148</v>
       </c>
@@ -3358,6 +3361,124 @@
       <c r="N86" s="14" t="n">
         <f aca="false">(L86-80000000)/80000000</f>
         <v>-0.607320831134565</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A88" s="16" t="n">
+        <v>45971</v>
+      </c>
+      <c r="B88" s="17"/>
+      <c r="C88" s="18" t="n">
+        <v>4</v>
+      </c>
+      <c r="D88" s="19" t="n">
+        <v>206603</v>
+      </c>
+      <c r="E88" s="20" t="n">
+        <v>199</v>
+      </c>
+      <c r="F88" s="19" t="n">
+        <f aca="false">D88/E88*1000</f>
+        <v>1038206.03015075</v>
+      </c>
+      <c r="G88" s="35" t="n">
+        <f aca="false">(E84-E88)/E84</f>
+        <v>0.0339805825242718</v>
+      </c>
+      <c r="H88" s="22" t="n">
+        <f aca="false">(F88-80000000)/80000000</f>
+        <v>-0.987022424623116</v>
+      </c>
+      <c r="I88" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="J88" s="19" t="n">
+        <v>197281</v>
+      </c>
+      <c r="K88" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="L88" s="19" t="n">
+        <f aca="false">J88/K88*1000</f>
+        <v>32880166.6666667</v>
+      </c>
+      <c r="M88" s="35" t="n">
+        <f aca="false">(K84-K88)/K84</f>
+        <v>0</v>
+      </c>
+      <c r="N88" s="22" t="n">
+        <f aca="false">(L88-80000000)/80000000</f>
+        <v>-0.588997916666667</v>
+      </c>
+      <c r="P88" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C89" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="D89" s="2" t="n">
+        <v>5072212</v>
+      </c>
+      <c r="E89" s="2" t="n">
+        <v>4875</v>
+      </c>
+      <c r="F89" s="12" t="n">
+        <f aca="false">D89/E89*1000</f>
+        <v>1040453.74358974</v>
+      </c>
+      <c r="G89" s="23" t="n">
+        <f aca="false">(E85-E89)/E85</f>
+        <v>0.0342709984152139</v>
+      </c>
+      <c r="H89" s="14" t="n">
+        <f aca="false">(F89-80000000)/80000000</f>
+        <v>-0.986994328205128</v>
+      </c>
+      <c r="I89" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="J89" s="12" t="n">
+        <v>4880523</v>
+      </c>
+      <c r="K89" s="2" t="n">
+        <v>155</v>
+      </c>
+      <c r="L89" s="12" t="n">
+        <f aca="false">J89/K89*1000</f>
+        <v>31487245.1612903</v>
+      </c>
+      <c r="M89" s="37" t="n">
+        <f aca="false">(K85-K89)/K85</f>
+        <v>0</v>
+      </c>
+      <c r="N89" s="14" t="n">
+        <f aca="false">(L89-80000000)/80000000</f>
+        <v>-0.606409435483871</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I90" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="J90" s="12" t="n">
+        <v>119060324</v>
+      </c>
+      <c r="K90" s="2" t="n">
+        <v>3798</v>
+      </c>
+      <c r="L90" s="12" t="n">
+        <f aca="false">J90/K90*1000</f>
+        <v>31348163.2438125</v>
+      </c>
+      <c r="M90" s="25" t="n">
+        <f aca="false">(K86-K90)/K86</f>
+        <v>-0.00211081794195251</v>
+      </c>
+      <c r="N90" s="14" t="n">
+        <f aca="false">(L90-80000000)/80000000</f>
+        <v>-0.608147959452343</v>
       </c>
     </row>
   </sheetData>
@@ -3399,13 +3520,13 @@
         <v>45393</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates test and performance test times after migration from fedora to mint
</commit_message>
<xml_diff>
--- a/docs/Performance.xlsx
+++ b/docs/Performance.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
   <si>
     <t xml:space="preserve">classic</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t xml:space="preserve">avoided obvious ray attacks calculation on verify checks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fedora to debian mint</t>
   </si>
   <si>
     <t xml:space="preserve">stockfish livello 1</t>
@@ -345,7 +348,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -495,6 +498,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="169" fontId="8" fillId="4" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -754,13 +761,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R90"/>
+  <dimension ref="A1:R94"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A42" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E89" activeCellId="0" sqref="E89"/>
+      <selection pane="topLeft" activeCell="J94" activeCellId="0" sqref="J94"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.1484375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="16.15234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="11.57"/>
@@ -3479,6 +3486,124 @@
       <c r="N90" s="14" t="n">
         <f aca="false">(L90-80000000)/80000000</f>
         <v>-0.608147959452343</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A92" s="16" t="n">
+        <v>45991</v>
+      </c>
+      <c r="B92" s="17"/>
+      <c r="C92" s="18" t="n">
+        <v>4</v>
+      </c>
+      <c r="D92" s="19" t="n">
+        <v>206603</v>
+      </c>
+      <c r="E92" s="20" t="n">
+        <v>207</v>
+      </c>
+      <c r="F92" s="19" t="n">
+        <f aca="false">D92/E92*1000</f>
+        <v>998082.125603865</v>
+      </c>
+      <c r="G92" s="24" t="n">
+        <f aca="false">(E88-E92)/E88</f>
+        <v>-0.0402010050251256</v>
+      </c>
+      <c r="H92" s="22" t="n">
+        <f aca="false">(F92-80000000)/80000000</f>
+        <v>-0.987523973429952</v>
+      </c>
+      <c r="I92" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="J92" s="19" t="n">
+        <v>197281</v>
+      </c>
+      <c r="K92" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="L92" s="19" t="n">
+        <f aca="false">J92/K92*1000</f>
+        <v>32880166.6666667</v>
+      </c>
+      <c r="M92" s="24" t="n">
+        <f aca="false">(K88-K92)/K88</f>
+        <v>0</v>
+      </c>
+      <c r="N92" s="22" t="n">
+        <f aca="false">(L92-80000000)/80000000</f>
+        <v>-0.588997916666667</v>
+      </c>
+      <c r="P92" s="38" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C93" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="D93" s="2" t="n">
+        <v>5072212</v>
+      </c>
+      <c r="E93" s="2" t="n">
+        <v>5126</v>
+      </c>
+      <c r="F93" s="12" t="n">
+        <f aca="false">D93/E93*1000</f>
+        <v>989506.827936013</v>
+      </c>
+      <c r="G93" s="25" t="n">
+        <f aca="false">(E89-E93)/E89</f>
+        <v>-0.0514871794871795</v>
+      </c>
+      <c r="H93" s="14" t="n">
+        <f aca="false">(F93-80000000)/80000000</f>
+        <v>-0.9876311646508</v>
+      </c>
+      <c r="I93" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="J93" s="12" t="n">
+        <v>4880523</v>
+      </c>
+      <c r="K93" s="2" t="n">
+        <v>167</v>
+      </c>
+      <c r="L93" s="12" t="n">
+        <f aca="false">J93/K93*1000</f>
+        <v>29224688.6227545</v>
+      </c>
+      <c r="M93" s="25" t="n">
+        <f aca="false">(K89-K93)/K89</f>
+        <v>-0.0774193548387097</v>
+      </c>
+      <c r="N93" s="14" t="n">
+        <f aca="false">(L93-80000000)/80000000</f>
+        <v>-0.634691392215569</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I94" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="J94" s="12" t="n">
+        <v>119060324</v>
+      </c>
+      <c r="K94" s="2" t="n">
+        <v>4097</v>
+      </c>
+      <c r="L94" s="12" t="n">
+        <f aca="false">J94/K94*1000</f>
+        <v>29060367.0978765</v>
+      </c>
+      <c r="M94" s="25" t="n">
+        <f aca="false">(K90-K94)/K90</f>
+        <v>-0.078725645076356</v>
+      </c>
+      <c r="N94" s="14" t="n">
+        <f aca="false">(L94-80000000)/80000000</f>
+        <v>-0.636745411276544</v>
       </c>
     </row>
   </sheetData>
@@ -3507,7 +3632,7 @@
       <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.1484375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.15234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="8.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="16.43"/>
@@ -3516,17 +3641,17 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="38" t="n">
+      <c r="A1" s="39" t="n">
         <v>45393</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
introduced Zobrist key calculation updated performance values according to new hardware/software setup removed on the fly ray attacks calculation methods
</commit_message>
<xml_diff>
--- a/docs/Performance.xlsx
+++ b/docs/Performance.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="42">
   <si>
     <t xml:space="preserve">classic</t>
   </si>
@@ -132,6 +132,12 @@
   </si>
   <si>
     <t xml:space="preserve">fedora to debian mint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">changed board representation to the classic Little-Endian Rank-File Mapping</t>
+  </si>
+  <si>
+    <t xml:space="preserve">downgrade to 32GB of RAM with minor performance</t>
   </si>
   <si>
     <t xml:space="preserve">stockfish livello 1</t>
@@ -761,10 +767,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R94"/>
+  <dimension ref="A1:R98"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A42" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J94" activeCellId="0" sqref="J94"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A54" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P96" activeCellId="0" sqref="P96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.15234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3535,7 +3541,7 @@
         <f aca="false">(L92-80000000)/80000000</f>
         <v>-0.588997916666667</v>
       </c>
-      <c r="P92" s="38" t="s">
+      <c r="P92" s="7" t="s">
         <v>36</v>
       </c>
     </row>
@@ -3604,6 +3610,127 @@
       <c r="N94" s="14" t="n">
         <f aca="false">(L94-80000000)/80000000</f>
         <v>-0.636745411276544</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="16" t="n">
+        <v>46027</v>
+      </c>
+      <c r="B96" s="17"/>
+      <c r="C96" s="18" t="n">
+        <v>4</v>
+      </c>
+      <c r="D96" s="19" t="n">
+        <v>206603</v>
+      </c>
+      <c r="E96" s="20" t="n">
+        <v>218</v>
+      </c>
+      <c r="F96" s="19" t="n">
+        <f aca="false">D96/E96*1000</f>
+        <v>947720.183486239</v>
+      </c>
+      <c r="G96" s="24" t="n">
+        <f aca="false">(E92-E96)/E92</f>
+        <v>-0.0531400966183575</v>
+      </c>
+      <c r="H96" s="22" t="n">
+        <f aca="false">(F96-80000000)/80000000</f>
+        <v>-0.988153497706422</v>
+      </c>
+      <c r="I96" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="J96" s="19" t="n">
+        <v>197281</v>
+      </c>
+      <c r="K96" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="L96" s="19" t="n">
+        <f aca="false">J96/K96*1000</f>
+        <v>28183000</v>
+      </c>
+      <c r="M96" s="24" t="n">
+        <f aca="false">(K92-K96)/K92</f>
+        <v>-0.166666666666667</v>
+      </c>
+      <c r="N96" s="22" t="n">
+        <f aca="false">(L96-80000000)/80000000</f>
+        <v>-0.6477125</v>
+      </c>
+      <c r="P96" s="38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C97" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="D97" s="2" t="n">
+        <v>5072212</v>
+      </c>
+      <c r="E97" s="2" t="n">
+        <v>5403</v>
+      </c>
+      <c r="F97" s="12" t="n">
+        <f aca="false">D97/E97*1000</f>
+        <v>938776.975754211</v>
+      </c>
+      <c r="G97" s="25" t="n">
+        <f aca="false">(E93-E97)/E93</f>
+        <v>-0.0540382364416699</v>
+      </c>
+      <c r="H97" s="14" t="n">
+        <f aca="false">(F97-80000000)/80000000</f>
+        <v>-0.988265287803072</v>
+      </c>
+      <c r="I97" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="J97" s="12" t="n">
+        <v>4880523</v>
+      </c>
+      <c r="K97" s="2" t="n">
+        <v>170</v>
+      </c>
+      <c r="L97" s="12" t="n">
+        <f aca="false">J97/K97*1000</f>
+        <v>28708958.8235294</v>
+      </c>
+      <c r="M97" s="25" t="n">
+        <f aca="false">(K93-K97)/K93</f>
+        <v>-0.0179640718562874</v>
+      </c>
+      <c r="N97" s="14" t="n">
+        <f aca="false">(L97-80000000)/80000000</f>
+        <v>-0.641138014705882</v>
+      </c>
+      <c r="P97" s="38" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I98" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="J98" s="12" t="n">
+        <v>119060324</v>
+      </c>
+      <c r="K98" s="2" t="n">
+        <v>4295</v>
+      </c>
+      <c r="L98" s="12" t="n">
+        <f aca="false">J98/K98*1000</f>
+        <v>27720680.7916182</v>
+      </c>
+      <c r="M98" s="25" t="n">
+        <f aca="false">(K94-K98)/K94</f>
+        <v>-0.0483280449109104</v>
+      </c>
+      <c r="N98" s="14" t="n">
+        <f aca="false">(L98-80000000)/80000000</f>
+        <v>-0.653491490104773</v>
       </c>
     </row>
   </sheetData>
@@ -3645,13 +3772,13 @@
         <v>45393</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added transposition table instead of moves cache using zobrist key refactored cmakelists.txt
</commit_message>
<xml_diff>
--- a/docs/Performance.xlsx
+++ b/docs/Performance.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
   <si>
     <t xml:space="preserve">classic</t>
   </si>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t xml:space="preserve">downgrade to 32GB of RAM with minor performance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Replaced cache with transposition table with Zobrist key</t>
   </si>
   <si>
     <t xml:space="preserve">stockfish livello 1</t>
@@ -767,10 +770,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R98"/>
+  <dimension ref="A1:R103"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A54" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P96" activeCellId="0" sqref="P96"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A56" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L103" activeCellId="0" sqref="L103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.15234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3659,7 +3662,7 @@
         <f aca="false">(L96-80000000)/80000000</f>
         <v>-0.6477125</v>
       </c>
-      <c r="P96" s="38" t="s">
+      <c r="P96" s="7" t="s">
         <v>37</v>
       </c>
     </row>
@@ -3706,7 +3709,7 @@
         <f aca="false">(L97-80000000)/80000000</f>
         <v>-0.641138014705882</v>
       </c>
-      <c r="P97" s="38" t="s">
+      <c r="P97" s="7" t="s">
         <v>38</v>
       </c>
     </row>
@@ -3731,6 +3734,162 @@
       <c r="N98" s="14" t="n">
         <f aca="false">(L98-80000000)/80000000</f>
         <v>-0.653491490104773</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="16" t="n">
+        <v>46040</v>
+      </c>
+      <c r="B100" s="27"/>
+      <c r="C100" s="28" t="n">
+        <v>4</v>
+      </c>
+      <c r="D100" s="29" t="n">
+        <v>206603</v>
+      </c>
+      <c r="E100" s="30" t="n">
+        <v>196</v>
+      </c>
+      <c r="F100" s="29" t="n">
+        <f aca="false">D100/E100*1000</f>
+        <v>1054096.93877551</v>
+      </c>
+      <c r="G100" s="35" t="n">
+        <f aca="false">(E96-E100)/E96</f>
+        <v>0.100917431192661</v>
+      </c>
+      <c r="H100" s="22" t="n">
+        <f aca="false">(F100-80000000)/80000000</f>
+        <v>-0.986823788265306</v>
+      </c>
+      <c r="I100" s="31" t="n">
+        <v>4</v>
+      </c>
+      <c r="J100" s="29" t="n">
+        <v>197281</v>
+      </c>
+      <c r="K100" s="31" t="n">
+        <v>7</v>
+      </c>
+      <c r="L100" s="29" t="n">
+        <f aca="false">J100/K100*1000</f>
+        <v>28183000</v>
+      </c>
+      <c r="M100" s="35" t="n">
+        <f aca="false">(K96-K100)/K96</f>
+        <v>0</v>
+      </c>
+      <c r="N100" s="22" t="n">
+        <f aca="false">(L100-80000000)/80000000</f>
+        <v>-0.6477125</v>
+      </c>
+      <c r="P100" s="38" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="32"/>
+      <c r="B101" s="33"/>
+      <c r="C101" s="32" t="n">
+        <v>5</v>
+      </c>
+      <c r="D101" s="32" t="n">
+        <v>5072212</v>
+      </c>
+      <c r="E101" s="32" t="n">
+        <v>4121</v>
+      </c>
+      <c r="F101" s="34" t="n">
+        <f aca="false">D101/E101*1000</f>
+        <v>1230820.67459355</v>
+      </c>
+      <c r="G101" s="23" t="n">
+        <f aca="false">(E97-E101)/E97</f>
+        <v>0.237275587636498</v>
+      </c>
+      <c r="H101" s="14" t="n">
+        <f aca="false">(F101-80000000)/80000000</f>
+        <v>-0.984614741567581</v>
+      </c>
+      <c r="I101" s="32" t="n">
+        <v>5</v>
+      </c>
+      <c r="J101" s="34" t="n">
+        <v>4880523</v>
+      </c>
+      <c r="K101" s="32" t="n">
+        <v>145</v>
+      </c>
+      <c r="L101" s="34" t="n">
+        <f aca="false">J101/K101*1000</f>
+        <v>33658779.3103448</v>
+      </c>
+      <c r="M101" s="37" t="n">
+        <f aca="false">(K97-K101)/K97</f>
+        <v>0.147058823529412</v>
+      </c>
+      <c r="N101" s="14" t="n">
+        <f aca="false">(L101-80000000)/80000000</f>
+        <v>-0.57926525862069</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="32"/>
+      <c r="B102" s="33"/>
+      <c r="C102" s="32"/>
+      <c r="D102" s="32"/>
+      <c r="E102" s="32"/>
+      <c r="F102" s="32"/>
+      <c r="G102" s="32"/>
+      <c r="H102" s="33"/>
+      <c r="I102" s="32" t="n">
+        <v>6</v>
+      </c>
+      <c r="J102" s="34" t="n">
+        <v>119060324</v>
+      </c>
+      <c r="K102" s="32" t="n">
+        <v>3136</v>
+      </c>
+      <c r="L102" s="34" t="n">
+        <f aca="false">J102/K102*1000</f>
+        <v>37965664.5408163</v>
+      </c>
+      <c r="M102" s="23" t="n">
+        <f aca="false">(K98-K102)/K98</f>
+        <v>0.269848661233993</v>
+      </c>
+      <c r="N102" s="14" t="n">
+        <f aca="false">(L102-80000000)/80000000</f>
+        <v>-0.525429193239796</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="32"/>
+      <c r="B103" s="33"/>
+      <c r="C103" s="32"/>
+      <c r="D103" s="32"/>
+      <c r="E103" s="32"/>
+      <c r="F103" s="32"/>
+      <c r="G103" s="32"/>
+      <c r="H103" s="33"/>
+      <c r="I103" s="32" t="n">
+        <v>7</v>
+      </c>
+      <c r="J103" s="34" t="n">
+        <v>3195901860</v>
+      </c>
+      <c r="K103" s="32" t="n">
+        <v>69384</v>
+      </c>
+      <c r="L103" s="34" t="n">
+        <f aca="false">J103/K103*1000</f>
+        <v>46061078.3465929</v>
+      </c>
+      <c r="M103" s="32"/>
+      <c r="N103" s="25" t="n">
+        <f aca="false">(L103-80000000)/80000000</f>
+        <v>-0.424236520667589</v>
       </c>
     </row>
   </sheetData>
@@ -3772,13 +3931,13 @@
         <v>45393</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
embedded array pool into transposition table added transposition table to perft definitely
</commit_message>
<xml_diff>
--- a/docs/Performance.xlsx
+++ b/docs/Performance.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
   <si>
     <t xml:space="preserve">classic</t>
   </si>
@@ -141,6 +141,9 @@
   </si>
   <si>
     <t xml:space="preserve">Replaced cache with transposition table with Zobrist key</t>
+  </si>
+  <si>
+    <t xml:space="preserve">added transposition table definitely</t>
   </si>
   <si>
     <t xml:space="preserve">stockfish livello 1</t>
@@ -770,10 +773,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R103"/>
+  <dimension ref="A1:R107"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A56" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L103" activeCellId="0" sqref="L103"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A65" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M109" activeCellId="0" sqref="M109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.15234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3783,7 +3786,7 @@
         <f aca="false">(L100-80000000)/80000000</f>
         <v>-0.6477125</v>
       </c>
-      <c r="P100" s="38" t="s">
+      <c r="P100" s="7" t="s">
         <v>39</v>
       </c>
     </row>
@@ -3890,6 +3893,124 @@
       <c r="N103" s="25" t="n">
         <f aca="false">(L103-80000000)/80000000</f>
         <v>-0.424236520667589</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="16" t="n">
+        <v>46049</v>
+      </c>
+      <c r="B105" s="17"/>
+      <c r="C105" s="18" t="n">
+        <v>4</v>
+      </c>
+      <c r="D105" s="19" t="n">
+        <v>206603</v>
+      </c>
+      <c r="E105" s="20" t="n">
+        <v>169</v>
+      </c>
+      <c r="F105" s="19" t="n">
+        <f aca="false">D105/E105*1000</f>
+        <v>1222502.95857988</v>
+      </c>
+      <c r="G105" s="35" t="n">
+        <f aca="false">(E96-E105)/E96</f>
+        <v>0.224770642201835</v>
+      </c>
+      <c r="H105" s="22" t="n">
+        <f aca="false">(F105-80000000)/80000000</f>
+        <v>-0.984718713017752</v>
+      </c>
+      <c r="I105" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="J105" s="19" t="n">
+        <v>197281</v>
+      </c>
+      <c r="K105" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="L105" s="19" t="n">
+        <f aca="false">J105/K105*1000</f>
+        <v>28183000</v>
+      </c>
+      <c r="M105" s="35" t="n">
+        <f aca="false">(K96-K105)/K96</f>
+        <v>0</v>
+      </c>
+      <c r="N105" s="22" t="n">
+        <f aca="false">(L105-80000000)/80000000</f>
+        <v>-0.6477125</v>
+      </c>
+      <c r="P105" s="38" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C106" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="D106" s="2" t="n">
+        <v>5072212</v>
+      </c>
+      <c r="E106" s="2" t="n">
+        <v>3708</v>
+      </c>
+      <c r="F106" s="12" t="n">
+        <f aca="false">D106/E106*1000</f>
+        <v>1367910.46386192</v>
+      </c>
+      <c r="G106" s="23" t="n">
+        <f aca="false">(E97-E106)/E97</f>
+        <v>0.313714602998334</v>
+      </c>
+      <c r="H106" s="14" t="n">
+        <f aca="false">(F106-80000000)/80000000</f>
+        <v>-0.982901119201726</v>
+      </c>
+      <c r="I106" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="J106" s="12" t="n">
+        <v>4880523</v>
+      </c>
+      <c r="K106" s="2" t="n">
+        <v>121</v>
+      </c>
+      <c r="L106" s="12" t="n">
+        <f aca="false">J106/K106*1000</f>
+        <v>40334900.8264463</v>
+      </c>
+      <c r="M106" s="23" t="n">
+        <f aca="false">(K97-K106)/K97</f>
+        <v>0.288235294117647</v>
+      </c>
+      <c r="N106" s="14" t="n">
+        <f aca="false">(L106-80000000)/80000000</f>
+        <v>-0.495813739669422</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I107" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="J107" s="12" t="n">
+        <v>119060324</v>
+      </c>
+      <c r="K107" s="2" t="n">
+        <v>2626</v>
+      </c>
+      <c r="L107" s="12" t="n">
+        <f aca="false">J107/K107*1000</f>
+        <v>45339041.8888043</v>
+      </c>
+      <c r="M107" s="23" t="n">
+        <f aca="false">(K98-K107)/K98</f>
+        <v>0.388591385331781</v>
+      </c>
+      <c r="N107" s="14" t="n">
+        <f aca="false">(L107-80000000)/80000000</f>
+        <v>-0.433261976389947</v>
       </c>
     </row>
   </sheetData>
@@ -3931,13 +4052,13 @@
         <v>45393</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some refactoring in generate moves returns added compiler flags
</commit_message>
<xml_diff>
--- a/docs/Performance.xlsx
+++ b/docs/Performance.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="45">
   <si>
     <t xml:space="preserve">classic</t>
   </si>
@@ -144,6 +144,9 @@
   </si>
   <si>
     <t xml:space="preserve">added transposition table definitely</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Improved compilation flags</t>
   </si>
   <si>
     <t xml:space="preserve">stockfish livello 1</t>
@@ -773,10 +776,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R107"/>
+  <dimension ref="A1:R111"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A65" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M109" activeCellId="0" sqref="M109"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A73" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E110" activeCellId="0" sqref="E110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.15234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3942,7 +3945,7 @@
         <f aca="false">(L105-80000000)/80000000</f>
         <v>-0.6477125</v>
       </c>
-      <c r="P105" s="38" t="s">
+      <c r="P105" s="7" t="s">
         <v>40</v>
       </c>
     </row>
@@ -4011,6 +4014,124 @@
       <c r="N107" s="14" t="n">
         <f aca="false">(L107-80000000)/80000000</f>
         <v>-0.433261976389947</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="16" t="n">
+        <v>46065</v>
+      </c>
+      <c r="B109" s="17"/>
+      <c r="C109" s="18" t="n">
+        <v>4</v>
+      </c>
+      <c r="D109" s="19" t="n">
+        <v>206603</v>
+      </c>
+      <c r="E109" s="20" t="n">
+        <v>147</v>
+      </c>
+      <c r="F109" s="19" t="n">
+        <f aca="false">D109/E109*1000</f>
+        <v>1405462.58503401</v>
+      </c>
+      <c r="G109" s="35" t="n">
+        <f aca="false">(E100-E109)/E100</f>
+        <v>0.25</v>
+      </c>
+      <c r="H109" s="22" t="n">
+        <f aca="false">(F109-80000000)/80000000</f>
+        <v>-0.982431717687075</v>
+      </c>
+      <c r="I109" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="J109" s="19" t="n">
+        <v>197281</v>
+      </c>
+      <c r="K109" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="L109" s="19" t="n">
+        <f aca="false">J109/K109*1000</f>
+        <v>32880166.6666667</v>
+      </c>
+      <c r="M109" s="35" t="n">
+        <f aca="false">(K100-K109)/K100</f>
+        <v>0.142857142857143</v>
+      </c>
+      <c r="N109" s="22" t="n">
+        <f aca="false">(L109-80000000)/80000000</f>
+        <v>-0.588997916666667</v>
+      </c>
+      <c r="P109" s="38" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C110" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="D110" s="2" t="n">
+        <v>5072212</v>
+      </c>
+      <c r="E110" s="2" t="n">
+        <v>3204</v>
+      </c>
+      <c r="F110" s="12" t="n">
+        <f aca="false">D110/E110*1000</f>
+        <v>1583087.39076155</v>
+      </c>
+      <c r="G110" s="23" t="n">
+        <f aca="false">(E101-E110)/E101</f>
+        <v>0.222518806115021</v>
+      </c>
+      <c r="H110" s="14" t="n">
+        <f aca="false">(F110-80000000)/80000000</f>
+        <v>-0.980211407615481</v>
+      </c>
+      <c r="I110" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="J110" s="12" t="n">
+        <v>4880523</v>
+      </c>
+      <c r="K110" s="2" t="n">
+        <v>115</v>
+      </c>
+      <c r="L110" s="12" t="n">
+        <f aca="false">J110/K110*1000</f>
+        <v>42439330.4347826</v>
+      </c>
+      <c r="M110" s="23" t="n">
+        <f aca="false">(K101-K110)/K101</f>
+        <v>0.206896551724138</v>
+      </c>
+      <c r="N110" s="14" t="n">
+        <f aca="false">(L110-80000000)/80000000</f>
+        <v>-0.469508369565217</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I111" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="J111" s="12" t="n">
+        <v>119060324</v>
+      </c>
+      <c r="K111" s="2" t="n">
+        <v>2536</v>
+      </c>
+      <c r="L111" s="12" t="n">
+        <f aca="false">J111/K111*1000</f>
+        <v>46948077.2870663</v>
+      </c>
+      <c r="M111" s="23" t="n">
+        <f aca="false">(K102-K111)/K102</f>
+        <v>0.191326530612245</v>
+      </c>
+      <c r="N111" s="14" t="n">
+        <f aca="false">(L111-80000000)/80000000</f>
+        <v>-0.413149033911672</v>
       </c>
     </row>
   </sheetData>
@@ -4052,13 +4173,13 @@
         <v>45393</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>